<commit_message>
Added filled daily template
</commit_message>
<xml_diff>
--- a/Inputs/WeeklyTemplates/2024 First half/Tuesday.xlsx
+++ b/Inputs/WeeklyTemplates/2024 First half/Tuesday.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ericl\OneDrive\Desktop\CDEV3300-Gate-Gourmet-Scheduling\Inputs\WeeklyTemplates\2024 First half\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2024project Tokyo\UNSW AI schedule project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE17CE20-122C-474B-AA78-4EFFEB5335B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA3E962-2A6C-4687-82EF-38508E33EDB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{8740E76B-EDAF-2240-BEB8-3D4AC43AF0EB}"/>
+    <workbookView xWindow="4777" yWindow="0" windowWidth="19306" windowHeight="15082" xr2:uid="{8740E76B-EDAF-2240-BEB8-3D4AC43AF0EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,28 +36,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="128">
-  <si>
-    <t>UA6 LD</t>
-  </si>
-  <si>
-    <t>LX161 PS / LD</t>
-  </si>
-  <si>
-    <t>TG ADD/UAICE</t>
-  </si>
-  <si>
-    <t>UA873OFLD</t>
-  </si>
-  <si>
-    <t>WS81PS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="164">
   <si>
     <t>無線機</t>
     <rPh sb="0" eb="3">
       <t>ムセンキ</t>
     </rPh>
     <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>Task Requirement</t>
+  </si>
+  <si>
+    <t>Duration</t>
   </si>
   <si>
     <r>
@@ -109,6 +100,12 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>IJ LD;LD</t>
+  </si>
+  <si>
+    <t>04:00-15:30</t>
+  </si>
+  <si>
     <t>TK51 LD</t>
     <phoneticPr fontId="0"/>
   </si>
@@ -128,6 +125,10 @@
   </si>
   <si>
     <t>APPIRE LOUNGE</t>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>TKKIT</t>
     <phoneticPr fontId="0"/>
   </si>
   <si>
@@ -154,11 +155,24 @@
     </r>
   </si>
   <si>
+    <t>UA6 LD</t>
+  </si>
+  <si>
+    <t>LD</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
+    <t>05:30-16:30</t>
+  </si>
+  <si>
     <t>温度計　13</t>
     <rPh sb="0" eb="3">
       <t>オンドケイ</t>
     </rPh>
     <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>LX161 PS / LD</t>
   </si>
   <si>
     <r>
@@ -188,6 +202,12 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>LX PS;LD</t>
+  </si>
+  <si>
+    <t>05:00-16:30</t>
+  </si>
+  <si>
     <t>TK51 PS / LD</t>
     <phoneticPr fontId="0"/>
   </si>
@@ -228,6 +248,12 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>TK PS;LD</t>
+  </si>
+  <si>
+    <t>06:00-17:00</t>
+  </si>
+  <si>
     <t>TG643PS / TG643 LD</t>
     <phoneticPr fontId="0"/>
   </si>
@@ -236,6 +262,12 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>TG PS;LD</t>
+  </si>
+  <si>
+    <t>08:00-17:30</t>
+  </si>
+  <si>
     <t xml:space="preserve"> TG643 LD / ICE</t>
   </si>
   <si>
@@ -243,10 +275,18 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>09:00-18:00</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t>QF80 LD</t>
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>09:00-20:30</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">UA838 LD </t>
     <phoneticPr fontId="0"/>
   </si>
@@ -261,6 +301,10 @@
   <si>
     <t>QF62 LD</t>
     <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>12:30-20:30</t>
+    <phoneticPr fontId="44" type="noConversion"/>
   </si>
   <si>
     <t>LX161 LD</t>
@@ -291,12 +335,27 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>TG ADD/UAICE</t>
+  </si>
+  <si>
     <t>JX805 LD</t>
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>08:00-20:30</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t>OM502 PS / LD</t>
     <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>OM PS;IJ LD</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
+    <t>07:30-16:30</t>
+    <phoneticPr fontId="44" type="noConversion"/>
   </si>
   <si>
     <t>トラック R2</t>
@@ -319,6 +378,10 @@
     </r>
   </si>
   <si>
+    <t>08:00-17:30</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">UA827 PS / LD    TG / LX / TK ADD </t>
     <phoneticPr fontId="0"/>
   </si>
@@ -327,6 +390,14 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>UA PS;LD</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
+    <t>08:00-18:00</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t>UA C/CK</t>
     <phoneticPr fontId="0"/>
   </si>
@@ -347,6 +418,10 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>06:30-18:00</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t>UA6C CK` UA841/ MEAL CK`</t>
     <phoneticPr fontId="0"/>
   </si>
@@ -367,12 +442,23 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>09:30-21:00</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t>UA33C CK` / MEAL CK`</t>
     <phoneticPr fontId="0"/>
   </si>
   <si>
     <t>UA33 PS / LD</t>
     <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>UA873OFLD</t>
+  </si>
+  <si>
+    <t>10:00-21:00</t>
+    <phoneticPr fontId="44" type="noConversion"/>
   </si>
   <si>
     <t>UA838 PS / LD</t>
@@ -394,6 +480,10 @@
     </r>
   </si>
   <si>
+    <t>06:30-17:30</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t>UA78C CK` / MEAL CK`</t>
     <phoneticPr fontId="0"/>
   </si>
@@ -406,6 +496,10 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>10:00-18:00</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t>HX607LD</t>
     <phoneticPr fontId="0"/>
   </si>
@@ -418,6 +512,14 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>JX PS;LD</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
+    <t>07:30-20:30</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t>HU440 PS / LD</t>
     <phoneticPr fontId="0"/>
   </si>
@@ -430,10 +532,29 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>HU PS;EK PS</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:30-23:00</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
+    <t>WS81PS</t>
+  </si>
+  <si>
     <t>WS81PS / LD</t>
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>WS PS;LD</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
+    <t>11:00-21:00</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t>HU440 LD</t>
     <phoneticPr fontId="0"/>
   </si>
@@ -446,6 +567,10 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>11:00-21:30</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t>HU7928 PS / LD</t>
     <phoneticPr fontId="0"/>
   </si>
@@ -458,12 +583,28 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>HU PS;LD</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
+    <t>11:30-21:00</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t>JX801 LD</t>
     <phoneticPr fontId="0"/>
   </si>
   <si>
     <t>QF62 PS / LD</t>
     <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>QF PS;LD</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
+    <t>11:30-22:00</t>
+    <phoneticPr fontId="44" type="noConversion"/>
   </si>
   <si>
     <t>QF80 PS / LD</t>
@@ -496,6 +637,10 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>12:00-21:30</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t>EKSUB CK</t>
     <phoneticPr fontId="0"/>
   </si>
@@ -514,6 +659,14 @@
   <si>
     <t>EK319 SUB / LD</t>
     <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>EK SUB;LD</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
+    <t>12:00-22:30</t>
+    <phoneticPr fontId="44" type="noConversion"/>
   </si>
   <si>
     <t>JX803 PS / LD</t>
@@ -543,6 +696,10 @@
     </r>
   </si>
   <si>
+    <t>12:30-22:30</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t>HX607PS / LD</t>
     <phoneticPr fontId="0"/>
   </si>
@@ -555,10 +712,22 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>06:30-14:30</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t>OS52 PS / LD</t>
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>OS PS;LD</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
+    <t>06:30-17:00</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t>TG677LD SUPPORT</t>
     <phoneticPr fontId="0"/>
   </si>
@@ -567,8 +736,20 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
+    <t>LO PS;LD</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
+    <t>13:30-23:00</t>
+    <phoneticPr fontId="44" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">UA33 LD </t>
     <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>12:30-21:00</t>
+    <phoneticPr fontId="44" type="noConversion"/>
   </si>
   <si>
     <t>HX605LD</t>
@@ -597,6 +778,10 @@
   <si>
     <t>EK319 LD/IJ001LD</t>
     <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>12:30-21:30</t>
+    <phoneticPr fontId="44" type="noConversion"/>
   </si>
   <si>
     <t>Alcohol</t>
@@ -667,61 +852,22 @@
     <t>Total work Hour</t>
     <phoneticPr fontId="0"/>
   </si>
-  <si>
-    <t>IJ LD;LD</t>
-  </si>
-  <si>
-    <t>LX PS;LD</t>
-  </si>
-  <si>
-    <t>TK PS;LD</t>
-  </si>
-  <si>
-    <t>TG PS;LD</t>
-  </si>
-  <si>
-    <t>Task Requirement</t>
-  </si>
-  <si>
-    <t>Duration</t>
-  </si>
-  <si>
-    <t>04:00-15:30</t>
-  </si>
-  <si>
-    <t>05:30-16:30</t>
-  </si>
-  <si>
-    <t>05:00-16:30</t>
-  </si>
-  <si>
-    <t>06:00-17:00</t>
-  </si>
-  <si>
-    <t>08:00-17:30</t>
-  </si>
-  <si>
-    <t>LD</t>
-  </si>
-  <si>
-    <t>TKKIT</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="0.00_ "/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.00_ "/>
     <numFmt numFmtId="166" formatCode="#,##0.00_ "/>
     <numFmt numFmtId="167" formatCode="0.0_ "/>
   </numFmts>
-  <fonts count="44">
+  <fonts count="45">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1010,6 +1156,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2060,7 +2213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="272">
+  <cellXfs count="273">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2284,27 +2437,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="35" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="35" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="38" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2323,37 +2476,37 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="2" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2396,8 +2549,8 @@
     <xf numFmtId="0" fontId="30" fillId="2" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="35" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2418,6 +2571,61 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="43" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="39" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="39" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="39" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2442,67 +2650,13 @@
     <xf numFmtId="167" fontId="39" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3135,166 +3289,166 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407072A9-3406-3A4A-863F-47DC030259EB}">
   <dimension ref="A1:CP86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CF1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="AO6" sqref="AO6"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="20" zoomScaleNormal="20" workbookViewId="0">
+      <selection activeCell="CM72" sqref="CM72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="29.5"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="29.65"/>
   <cols>
-    <col min="93" max="94" width="44.83203125" style="242" customWidth="1"/>
+    <col min="93" max="94" width="44.875" style="242" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" ht="30.5" thickTop="1" thickBot="1">
+    <row r="1" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A1" s="215"/>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="268">
+      <c r="H1" s="244">
         <v>4</v>
       </c>
-      <c r="I1" s="271"/>
+      <c r="I1" s="245"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
-      <c r="L1" s="271">
+      <c r="L1" s="245">
         <v>5</v>
       </c>
-      <c r="M1" s="271"/>
+      <c r="M1" s="245"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
-      <c r="P1" s="271">
+      <c r="P1" s="245">
         <v>6</v>
       </c>
-      <c r="Q1" s="271"/>
+      <c r="Q1" s="245"/>
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
-      <c r="T1" s="271">
+      <c r="T1" s="245">
         <v>7</v>
       </c>
-      <c r="U1" s="271"/>
+      <c r="U1" s="245"/>
       <c r="V1" s="7"/>
       <c r="W1" s="7"/>
-      <c r="X1" s="271">
+      <c r="X1" s="245">
         <v>8</v>
       </c>
-      <c r="Y1" s="271"/>
+      <c r="Y1" s="245"/>
       <c r="Z1" s="7"/>
       <c r="AA1" s="7"/>
-      <c r="AB1" s="271">
+      <c r="AB1" s="245">
         <v>9</v>
       </c>
-      <c r="AC1" s="271"/>
+      <c r="AC1" s="245"/>
       <c r="AD1" s="7"/>
       <c r="AE1" s="7"/>
-      <c r="AF1" s="271">
+      <c r="AF1" s="245">
         <v>10</v>
       </c>
-      <c r="AG1" s="271"/>
+      <c r="AG1" s="245"/>
       <c r="AH1" s="7"/>
       <c r="AI1" s="7"/>
-      <c r="AJ1" s="271">
+      <c r="AJ1" s="245">
         <v>11</v>
       </c>
-      <c r="AK1" s="271"/>
+      <c r="AK1" s="245"/>
       <c r="AL1" s="7"/>
       <c r="AM1" s="7"/>
-      <c r="AN1" s="268">
+      <c r="AN1" s="244">
         <v>12</v>
       </c>
-      <c r="AO1" s="268"/>
+      <c r="AO1" s="244"/>
       <c r="AP1" s="8"/>
       <c r="AQ1" s="7"/>
-      <c r="AR1" s="271">
+      <c r="AR1" s="245">
         <v>13</v>
       </c>
-      <c r="AS1" s="271"/>
+      <c r="AS1" s="245"/>
       <c r="AT1" s="7"/>
       <c r="AU1" s="7"/>
-      <c r="AV1" s="271">
+      <c r="AV1" s="245">
         <v>14</v>
       </c>
-      <c r="AW1" s="271"/>
+      <c r="AW1" s="245"/>
       <c r="AX1" s="7"/>
       <c r="AY1" s="7"/>
-      <c r="AZ1" s="271">
+      <c r="AZ1" s="245">
         <v>15</v>
       </c>
-      <c r="BA1" s="271"/>
+      <c r="BA1" s="245"/>
       <c r="BB1" s="7"/>
       <c r="BC1" s="8"/>
-      <c r="BD1" s="268">
+      <c r="BD1" s="244">
         <v>16</v>
       </c>
-      <c r="BE1" s="268"/>
+      <c r="BE1" s="244"/>
       <c r="BF1" s="8"/>
       <c r="BG1" s="8"/>
-      <c r="BH1" s="268">
+      <c r="BH1" s="244">
         <v>17</v>
       </c>
-      <c r="BI1" s="268"/>
+      <c r="BI1" s="244"/>
       <c r="BJ1" s="8"/>
       <c r="BK1" s="7"/>
-      <c r="BL1" s="271">
+      <c r="BL1" s="245">
         <v>18</v>
       </c>
-      <c r="BM1" s="271"/>
+      <c r="BM1" s="245"/>
       <c r="BN1" s="7"/>
       <c r="BO1" s="7"/>
-      <c r="BP1" s="271">
+      <c r="BP1" s="245">
         <v>19</v>
       </c>
-      <c r="BQ1" s="271"/>
+      <c r="BQ1" s="245"/>
       <c r="BR1" s="7"/>
       <c r="BS1" s="7"/>
-      <c r="BT1" s="271">
+      <c r="BT1" s="245">
         <v>20</v>
       </c>
-      <c r="BU1" s="271"/>
+      <c r="BU1" s="245"/>
       <c r="BV1" s="7"/>
       <c r="BW1" s="7"/>
-      <c r="BX1" s="271">
+      <c r="BX1" s="245">
         <v>21</v>
       </c>
-      <c r="BY1" s="271"/>
+      <c r="BY1" s="245"/>
       <c r="BZ1" s="9"/>
       <c r="CA1" s="9"/>
-      <c r="CB1" s="271">
+      <c r="CB1" s="245">
         <v>22</v>
       </c>
-      <c r="CC1" s="271"/>
+      <c r="CC1" s="245"/>
       <c r="CD1" s="9"/>
       <c r="CE1" s="7"/>
-      <c r="CF1" s="271">
+      <c r="CF1" s="245">
         <v>23</v>
       </c>
-      <c r="CG1" s="271"/>
+      <c r="CG1" s="245"/>
       <c r="CH1" s="7"/>
       <c r="CI1" s="7"/>
-      <c r="CJ1" s="271">
+      <c r="CJ1" s="245">
         <v>24</v>
       </c>
-      <c r="CK1" s="271"/>
+      <c r="CK1" s="245"/>
       <c r="CL1" s="7"/>
       <c r="CM1" s="7"/>
       <c r="CN1" s="10"/>
       <c r="CO1" s="234" t="s">
-        <v>119</v>
+        <v>1</v>
       </c>
       <c r="CP1" s="234" t="s">
-        <v>120</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="2" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A2" s="216"/>
       <c r="B2" s="11">
         <v>3</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="14"/>
@@ -3303,7 +3457,7 @@
         <v>-7</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H2" s="17">
         <f>E3</f>
@@ -3311,14 +3465,14 @@
       </c>
       <c r="I2" s="18"/>
       <c r="J2" s="19" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K2" s="20"/>
       <c r="L2" s="21"/>
       <c r="M2" s="20"/>
       <c r="N2" s="21"/>
       <c r="O2" s="22" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
@@ -3333,7 +3487,7 @@
       <c r="Z2" s="26"/>
       <c r="AA2" s="21"/>
       <c r="AB2" s="27" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AC2" s="20"/>
       <c r="AD2" s="21"/>
@@ -3344,7 +3498,7 @@
       <c r="AI2" s="21"/>
       <c r="AJ2" s="21"/>
       <c r="AK2" s="28" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="AL2" s="21"/>
       <c r="AM2" s="24"/>
@@ -3355,12 +3509,12 @@
       <c r="AR2" s="21"/>
       <c r="AS2" s="20"/>
       <c r="AT2" s="29" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="AU2" s="20"/>
       <c r="AV2" s="21"/>
       <c r="AW2" s="30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="AX2" s="21"/>
       <c r="AY2" s="21"/>
@@ -3406,13 +3560,13 @@
       <c r="CM2" s="38"/>
       <c r="CN2" s="39"/>
       <c r="CO2" s="235" t="s">
-        <v>115</v>
+        <v>11</v>
       </c>
       <c r="CP2" s="235" t="s">
-        <v>121</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="3" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A3" s="217"/>
       <c r="B3" s="40"/>
       <c r="C3" s="41">
@@ -3592,13 +3746,13 @@
       <c r="CO3" s="236"/>
       <c r="CP3" s="236"/>
     </row>
-    <row r="4" spans="1:94" ht="30.5" thickBot="1">
+    <row r="4" spans="1:94" ht="30" thickBot="1">
       <c r="A4" s="216"/>
       <c r="B4" s="11">
         <v>4</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D4" s="59"/>
       <c r="E4" s="60"/>
@@ -3607,7 +3761,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H4" s="63">
         <f>E5</f>
@@ -3615,7 +3769,7 @@
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="19" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -3632,7 +3786,7 @@
       <c r="W4" s="24"/>
       <c r="X4" s="24"/>
       <c r="Y4" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Z4" s="19"/>
       <c r="AA4" s="21"/>
@@ -3644,7 +3798,7 @@
       <c r="AG4" s="21"/>
       <c r="AH4" s="21"/>
       <c r="AI4" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AJ4" s="23"/>
       <c r="AK4" s="24"/>
@@ -3657,12 +3811,12 @@
       <c r="AR4" s="21"/>
       <c r="AS4" s="20"/>
       <c r="AT4" s="29" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="AU4" s="20"/>
       <c r="AV4" s="21"/>
       <c r="AW4" s="30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="AX4" s="21"/>
       <c r="AY4" s="21"/>
@@ -3708,13 +3862,13 @@
       <c r="CM4" s="68"/>
       <c r="CN4" s="69"/>
       <c r="CO4" s="237" t="s">
-        <v>115</v>
+        <v>11</v>
       </c>
       <c r="CP4" s="237" t="s">
-        <v>121</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:94" ht="30.5" thickBot="1">
+    <row r="5" spans="1:94" ht="30" thickBot="1">
       <c r="A5" s="218"/>
       <c r="B5" s="40"/>
       <c r="C5" s="70">
@@ -3898,13 +4052,13 @@
       <c r="CO5" s="238"/>
       <c r="CP5" s="238"/>
     </row>
-    <row r="6" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="6" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A6" s="219"/>
       <c r="B6" s="80">
         <v>5</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D6" s="42"/>
       <c r="E6" s="13"/>
@@ -3913,14 +4067,14 @@
         <v>12</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H6" s="17">
         <f>E7</f>
         <v>2.5</v>
       </c>
       <c r="I6" s="81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" s="63"/>
       <c r="K6" s="82"/>
@@ -3931,7 +4085,7 @@
       <c r="N6" s="63"/>
       <c r="O6" s="84"/>
       <c r="P6" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q6" s="20"/>
       <c r="R6" s="21"/>
@@ -3940,12 +4094,12 @@
       <c r="U6" s="85"/>
       <c r="V6" s="24"/>
       <c r="W6" s="84" t="s">
-        <v>127</v>
+        <v>17</v>
       </c>
       <c r="X6" s="21"/>
       <c r="Y6" s="21"/>
       <c r="Z6" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AA6" s="21"/>
       <c r="AB6" s="21"/>
@@ -3973,12 +4127,12 @@
       <c r="AT6" s="21"/>
       <c r="AU6" s="18"/>
       <c r="AV6" s="29" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AW6" s="20"/>
       <c r="AX6" s="21"/>
       <c r="AY6" s="30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="AZ6" s="23"/>
       <c r="BA6" s="20"/>
@@ -4022,13 +4176,13 @@
       <c r="CM6" s="17"/>
       <c r="CN6" s="32"/>
       <c r="CO6" s="239" t="s">
-        <v>126</v>
+        <v>21</v>
       </c>
       <c r="CP6" s="239" t="s">
-        <v>122</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:94" ht="30.5" thickBot="1">
+    <row r="7" spans="1:94" ht="30" thickBot="1">
       <c r="A7" s="218"/>
       <c r="B7" s="11"/>
       <c r="C7" s="70">
@@ -4208,13 +4362,13 @@
       <c r="CO7" s="240"/>
       <c r="CP7" s="240"/>
     </row>
-    <row r="8" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="8" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A8" s="216"/>
       <c r="B8" s="80">
         <v>6</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D8" s="59"/>
       <c r="E8" s="60"/>
@@ -4223,14 +4377,14 @@
         <v>14</v>
       </c>
       <c r="G8" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H8" s="63">
         <f>E9</f>
         <v>3.5</v>
       </c>
       <c r="I8" s="81" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J8" s="17"/>
       <c r="K8" s="49"/>
@@ -4239,7 +4393,7 @@
       <c r="N8" s="21"/>
       <c r="O8" s="21"/>
       <c r="P8" s="27" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="Q8" s="20"/>
       <c r="R8" s="21"/>
@@ -4268,19 +4422,19 @@
       <c r="AO8" s="24"/>
       <c r="AP8" s="24"/>
       <c r="AQ8" s="91" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="AR8" s="23"/>
       <c r="AS8" s="20"/>
       <c r="AT8" s="21"/>
       <c r="AU8" s="18"/>
       <c r="AV8" s="29" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="AW8" s="20"/>
       <c r="AX8" s="21"/>
       <c r="AY8" s="30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="AZ8" s="23"/>
       <c r="BA8" s="20"/>
@@ -4324,13 +4478,13 @@
       <c r="CM8" s="68"/>
       <c r="CN8" s="69"/>
       <c r="CO8" s="234" t="s">
-        <v>116</v>
+        <v>27</v>
       </c>
       <c r="CP8" s="234" t="s">
-        <v>123</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:94" ht="30.5" thickBot="1">
+    <row r="9" spans="1:94" ht="30" thickBot="1">
       <c r="A9" s="217"/>
       <c r="B9" s="40"/>
       <c r="C9" s="70">
@@ -4518,7 +4672,7 @@
       <c r="CO9" s="238"/>
       <c r="CP9" s="238"/>
     </row>
-    <row r="10" spans="1:94" ht="36" thickTop="1" thickBot="1">
+    <row r="10" spans="1:94" ht="36.75" thickTop="1" thickBot="1">
       <c r="A10" s="216"/>
       <c r="B10" s="11">
         <v>7</v>
@@ -4531,14 +4685,14 @@
         <v>13</v>
       </c>
       <c r="G10" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H10" s="17">
         <f>E11</f>
         <v>3</v>
       </c>
       <c r="I10" s="81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J10" s="63"/>
       <c r="K10" s="82"/>
@@ -4551,7 +4705,7 @@
       <c r="P10" s="63"/>
       <c r="Q10" s="18"/>
       <c r="R10" s="27" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="S10" s="93"/>
       <c r="T10" s="23"/>
@@ -4578,7 +4732,7 @@
       <c r="AO10" s="24"/>
       <c r="AP10" s="24"/>
       <c r="AQ10" s="87" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="AR10" s="23"/>
       <c r="AS10" s="20"/>
@@ -4587,7 +4741,7 @@
       <c r="AV10" s="23"/>
       <c r="AW10" s="20"/>
       <c r="AX10" s="29" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="AY10" s="21"/>
       <c r="AZ10" s="21"/>
@@ -4595,7 +4749,7 @@
       <c r="BB10" s="21"/>
       <c r="BC10" s="18"/>
       <c r="BD10" s="29" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="BE10" s="20"/>
       <c r="BF10" s="21"/>
@@ -4634,13 +4788,13 @@
       <c r="CM10" s="17"/>
       <c r="CN10" s="32"/>
       <c r="CO10" s="239" t="s">
-        <v>117</v>
+        <v>33</v>
       </c>
       <c r="CP10" s="239" t="s">
-        <v>124</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:94" ht="30.5" thickBot="1">
+    <row r="11" spans="1:94" ht="30" thickBot="1">
       <c r="A11" s="217"/>
       <c r="B11" s="11"/>
       <c r="C11" s="41">
@@ -4824,7 +4978,7 @@
       <c r="CO11" s="240"/>
       <c r="CP11" s="240"/>
     </row>
-    <row r="12" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="12" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A12" s="218"/>
       <c r="B12" s="80">
         <v>8</v>
@@ -4837,14 +4991,14 @@
         <v>10</v>
       </c>
       <c r="G12" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H12" s="63">
         <f>E13</f>
         <v>1.5</v>
       </c>
       <c r="I12" s="81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J12" s="63"/>
       <c r="K12" s="82"/>
@@ -4872,7 +5026,7 @@
       <c r="AE12" s="21"/>
       <c r="AF12" s="21"/>
       <c r="AG12" s="19" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="AH12" s="21"/>
       <c r="AI12" s="19"/>
@@ -4893,7 +5047,7 @@
       <c r="AX12" s="21"/>
       <c r="AY12" s="30"/>
       <c r="AZ12" s="19" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="BA12" s="20"/>
       <c r="BB12" s="19"/>
@@ -4936,13 +5090,13 @@
       <c r="CM12" s="95"/>
       <c r="CN12" s="99"/>
       <c r="CO12" s="234" t="s">
-        <v>118</v>
+        <v>37</v>
       </c>
       <c r="CP12" s="234" t="s">
-        <v>125</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:94" ht="30.5" thickBot="1">
+    <row r="13" spans="1:94" ht="30" thickBot="1">
       <c r="A13" s="217"/>
       <c r="B13" s="11"/>
       <c r="C13" s="100">
@@ -5114,7 +5268,7 @@
       <c r="CO13" s="238"/>
       <c r="CP13" s="238"/>
     </row>
-    <row r="14" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="14" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A14" s="218"/>
       <c r="B14" s="80">
         <v>9</v>
@@ -5127,14 +5281,14 @@
         <v>9</v>
       </c>
       <c r="G14" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H14" s="63">
         <f>E15</f>
         <v>1</v>
       </c>
       <c r="I14" s="102" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J14" s="17"/>
       <c r="K14" s="49"/>
@@ -5159,7 +5313,7 @@
       <c r="AB14" s="17"/>
       <c r="AC14" s="18"/>
       <c r="AD14" s="27" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="AE14" s="19"/>
       <c r="AF14" s="21"/>
@@ -5175,7 +5329,7 @@
       <c r="AP14" s="24"/>
       <c r="AQ14" s="87"/>
       <c r="AR14" s="27" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AS14" s="21"/>
       <c r="AT14" s="21"/>
@@ -5225,10 +5379,14 @@
       <c r="CL14" s="68"/>
       <c r="CM14" s="68"/>
       <c r="CN14" s="69"/>
-      <c r="CO14" s="234"/>
-      <c r="CP14" s="234"/>
+      <c r="CO14" s="234" t="s">
+        <v>21</v>
+      </c>
+      <c r="CP14" s="243" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="15" spans="1:94" ht="30.5" thickBot="1">
+    <row r="15" spans="1:94" ht="30" thickBot="1">
       <c r="A15" s="218"/>
       <c r="B15" s="40"/>
       <c r="C15" s="41">
@@ -5396,7 +5554,7 @@
       <c r="CO15" s="238"/>
       <c r="CP15" s="238"/>
     </row>
-    <row r="16" spans="1:94" ht="36" thickTop="1" thickBot="1">
+    <row r="16" spans="1:94" ht="36.75" thickTop="1" thickBot="1">
       <c r="A16" s="216"/>
       <c r="B16" s="104">
         <v>10</v>
@@ -5409,7 +5567,7 @@
         <v>12</v>
       </c>
       <c r="G16" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H16" s="63">
         <f>E17</f>
@@ -5437,7 +5595,7 @@
       <c r="AB16" s="63"/>
       <c r="AC16" s="18"/>
       <c r="AD16" s="27" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="AE16" s="19"/>
       <c r="AF16" s="21"/>
@@ -5452,7 +5610,7 @@
       <c r="AO16" s="24"/>
       <c r="AP16" s="24"/>
       <c r="AQ16" s="87" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="AR16" s="23"/>
       <c r="AS16" s="20"/>
@@ -5461,7 +5619,7 @@
       <c r="AV16" s="23"/>
       <c r="AW16" s="20"/>
       <c r="AX16" s="29" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="AY16" s="21"/>
       <c r="AZ16" s="21"/>
@@ -5469,7 +5627,7 @@
       <c r="BB16" s="21"/>
       <c r="BC16" s="18"/>
       <c r="BD16" s="29" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="BE16" s="20"/>
       <c r="BF16" s="21"/>
@@ -5481,7 +5639,7 @@
       <c r="BL16" s="24"/>
       <c r="BM16" s="105"/>
       <c r="BN16" s="19" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="BO16" s="105"/>
       <c r="BP16" s="105"/>
@@ -5509,10 +5667,14 @@
       <c r="CL16" s="95"/>
       <c r="CM16" s="95"/>
       <c r="CN16" s="99"/>
-      <c r="CO16" s="234"/>
-      <c r="CP16" s="234"/>
+      <c r="CO16" s="234" t="s">
+        <v>21</v>
+      </c>
+      <c r="CP16" s="234" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="17" spans="1:94" ht="30.5" thickBot="1">
+    <row r="17" spans="1:94" ht="30" thickBot="1">
       <c r="A17" s="217"/>
       <c r="B17" s="11"/>
       <c r="C17" s="70">
@@ -5692,7 +5854,7 @@
       <c r="CO17" s="238"/>
       <c r="CP17" s="238"/>
     </row>
-    <row r="18" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="18" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A18" s="216"/>
       <c r="B18" s="80">
         <v>11</v>
@@ -5705,7 +5867,7 @@
         <v>7</v>
       </c>
       <c r="G18" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H18" s="63">
         <f>E19</f>
@@ -5749,12 +5911,12 @@
       <c r="AR18" s="21"/>
       <c r="AS18" s="20"/>
       <c r="AT18" s="29" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="AU18" s="20"/>
       <c r="AV18" s="21"/>
       <c r="AW18" s="30" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="AX18" s="21"/>
       <c r="AY18" s="21"/>
@@ -5765,7 +5927,7 @@
       <c r="BD18" s="21"/>
       <c r="BE18" s="18"/>
       <c r="BF18" s="19" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="BG18" s="21"/>
       <c r="BH18" s="21"/>
@@ -5776,7 +5938,7 @@
       <c r="BM18" s="24"/>
       <c r="BN18" s="24"/>
       <c r="BO18" s="19" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="BP18" s="19"/>
       <c r="BQ18" s="21"/>
@@ -5803,10 +5965,14 @@
       <c r="CL18" s="95"/>
       <c r="CM18" s="95"/>
       <c r="CN18" s="99"/>
-      <c r="CO18" s="234"/>
-      <c r="CP18" s="234"/>
+      <c r="CO18" s="234" t="s">
+        <v>21</v>
+      </c>
+      <c r="CP18" s="234" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="19" spans="1:94" ht="30.5" thickBot="1">
+    <row r="19" spans="1:94" ht="30" thickBot="1">
       <c r="A19" s="218"/>
       <c r="B19" s="40"/>
       <c r="C19" s="100">
@@ -5966,7 +6132,7 @@
       <c r="CO19" s="238"/>
       <c r="CP19" s="238"/>
     </row>
-    <row r="20" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="20" spans="1:94" ht="30.75" thickTop="1" thickBot="1">
       <c r="A20" s="216"/>
       <c r="B20" s="11">
         <v>12</v>
@@ -5979,7 +6145,7 @@
         <v>15</v>
       </c>
       <c r="G20" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H20" s="63">
         <f>E21</f>
@@ -6005,7 +6171,7 @@
       <c r="Z20" s="19"/>
       <c r="AA20" s="21"/>
       <c r="AB20" s="27" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="AC20" s="20"/>
       <c r="AD20" s="21"/>
@@ -6013,7 +6179,7 @@
       <c r="AF20" s="21"/>
       <c r="AG20" s="110"/>
       <c r="AH20" s="19" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="AI20" s="19"/>
       <c r="AJ20" s="23"/>
@@ -6027,7 +6193,7 @@
       <c r="AR20" s="21"/>
       <c r="AS20" s="27"/>
       <c r="AT20" s="27" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="AU20" s="21"/>
       <c r="AV20" s="19"/>
@@ -6036,7 +6202,7 @@
       <c r="AY20" s="21"/>
       <c r="AZ20" s="21"/>
       <c r="BA20" s="111" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="BB20" s="20"/>
       <c r="BC20" s="21"/>
@@ -6044,7 +6210,7 @@
       <c r="BE20" s="30"/>
       <c r="BF20" s="23"/>
       <c r="BG20" s="4" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="BH20" s="27"/>
       <c r="BI20" s="21"/>
@@ -6053,7 +6219,7 @@
       <c r="BL20" s="112"/>
       <c r="BM20" s="105"/>
       <c r="BN20" s="19" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="BO20" s="105"/>
       <c r="BP20" s="105"/>
@@ -6081,10 +6247,14 @@
       <c r="CL20" s="68"/>
       <c r="CM20" s="68"/>
       <c r="CN20" s="69"/>
-      <c r="CO20" s="234"/>
-      <c r="CP20" s="234"/>
+      <c r="CO20" s="234" t="s">
+        <v>21</v>
+      </c>
+      <c r="CP20" s="234" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="21" spans="1:94" ht="30.5" thickBot="1">
+    <row r="21" spans="1:94" ht="30" thickBot="1">
       <c r="A21" s="217"/>
       <c r="B21" s="11"/>
       <c r="C21" s="70">
@@ -6276,7 +6446,7 @@
       <c r="CO21" s="238"/>
       <c r="CP21" s="238"/>
     </row>
-    <row r="22" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="22" spans="1:94" ht="30.75" thickTop="1" thickBot="1">
       <c r="A22" s="218"/>
       <c r="B22" s="80">
         <v>13</v>
@@ -6289,14 +6459,14 @@
         <v>9</v>
       </c>
       <c r="G22" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H22" s="17">
         <f>E23</f>
         <v>1</v>
       </c>
       <c r="I22" s="81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J22" s="63"/>
       <c r="K22" s="82"/>
@@ -6319,7 +6489,7 @@
       <c r="Z22" s="19"/>
       <c r="AA22" s="21"/>
       <c r="AB22" s="27" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="AC22" s="20"/>
       <c r="AD22" s="21"/>
@@ -6328,7 +6498,7 @@
       <c r="AG22" s="21"/>
       <c r="AH22" s="86"/>
       <c r="AI22" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AJ22" s="23"/>
       <c r="AK22" s="24"/>
@@ -6337,7 +6507,7 @@
       <c r="AN22" s="24"/>
       <c r="AO22" s="18"/>
       <c r="AP22" s="27" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="AQ22" s="21"/>
       <c r="AR22" s="19"/>
@@ -6352,7 +6522,7 @@
       <c r="BA22" s="21"/>
       <c r="BB22" s="21"/>
       <c r="BC22" s="111" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="BD22" s="21"/>
       <c r="BE22" s="111"/>
@@ -6391,10 +6561,14 @@
       <c r="CL22" s="68"/>
       <c r="CM22" s="68"/>
       <c r="CN22" s="69"/>
-      <c r="CO22" s="239"/>
-      <c r="CP22" s="239"/>
+      <c r="CO22" s="239" t="s">
+        <v>57</v>
+      </c>
+      <c r="CP22" s="239" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="23" spans="1:94" ht="30.5" thickBot="1">
+    <row r="23" spans="1:94" ht="30" thickBot="1">
       <c r="A23" s="218"/>
       <c r="B23" s="40"/>
       <c r="C23" s="41">
@@ -6562,7 +6736,7 @@
       <c r="CO23" s="240"/>
       <c r="CP23" s="240"/>
     </row>
-    <row r="24" spans="1:94" ht="36" thickTop="1" thickBot="1">
+    <row r="24" spans="1:94" ht="36.75" thickTop="1" thickBot="1">
       <c r="A24" s="216"/>
       <c r="B24" s="11">
         <v>14</v>
@@ -6575,7 +6749,7 @@
         <v>10</v>
       </c>
       <c r="G24" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H24" s="17">
         <f>E25</f>
@@ -6601,7 +6775,7 @@
       <c r="Z24" s="19"/>
       <c r="AA24" s="21"/>
       <c r="AB24" s="27" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="AC24" s="20"/>
       <c r="AD24" s="27"/>
@@ -6623,12 +6797,12 @@
       <c r="AR24" s="21"/>
       <c r="AS24" s="20"/>
       <c r="AT24" s="29" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="AU24" s="20"/>
       <c r="AV24" s="21"/>
       <c r="AW24" s="30" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="AX24" s="21"/>
       <c r="AY24" s="21"/>
@@ -6639,7 +6813,7 @@
       <c r="BD24" s="21"/>
       <c r="BE24" s="18"/>
       <c r="BF24" s="19" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="BG24" s="21"/>
       <c r="BH24" s="21"/>
@@ -6675,10 +6849,14 @@
       <c r="CL24" s="95"/>
       <c r="CM24" s="95"/>
       <c r="CN24" s="99"/>
-      <c r="CO24" s="239"/>
-      <c r="CP24" s="239"/>
+      <c r="CO24" s="239" t="s">
+        <v>21</v>
+      </c>
+      <c r="CP24" s="239" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="25" spans="1:94" ht="30.5" thickBot="1">
+    <row r="25" spans="1:94" ht="30" thickBot="1">
       <c r="A25" s="217"/>
       <c r="B25" s="115"/>
       <c r="C25" s="116">
@@ -6850,7 +7028,7 @@
       <c r="CO25" s="240"/>
       <c r="CP25" s="240"/>
     </row>
-    <row r="26" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="26" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A26" s="216"/>
       <c r="B26" s="80">
         <v>15</v>
@@ -6863,14 +7041,14 @@
         <v>11</v>
       </c>
       <c r="G26" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H26" s="63">
         <f>E27</f>
         <v>2</v>
       </c>
       <c r="I26" s="81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J26" s="63"/>
       <c r="K26" s="82"/>
@@ -6891,7 +7069,7 @@
       <c r="X26" s="63"/>
       <c r="Y26" s="18"/>
       <c r="Z26" s="27" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="AA26" s="21"/>
       <c r="AB26" s="23"/>
@@ -6911,7 +7089,7 @@
       <c r="AP26" s="24"/>
       <c r="AQ26" s="21"/>
       <c r="AR26" s="19" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="AS26" s="20"/>
       <c r="AT26" s="21"/>
@@ -6961,10 +7139,14 @@
       <c r="CL26" s="68"/>
       <c r="CM26" s="68"/>
       <c r="CN26" s="69"/>
-      <c r="CO26" s="234"/>
-      <c r="CP26" s="234"/>
+      <c r="CO26" s="234" t="s">
+        <v>64</v>
+      </c>
+      <c r="CP26" s="234" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="27" spans="1:94" ht="30.5" thickBot="1">
+    <row r="27" spans="1:94" ht="30" thickBot="1">
       <c r="A27" s="217"/>
       <c r="B27" s="40"/>
       <c r="C27" s="70">
@@ -7140,7 +7322,7 @@
       <c r="CO27" s="238"/>
       <c r="CP27" s="238"/>
     </row>
-    <row r="28" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="28" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A28" s="219"/>
       <c r="B28" s="80">
         <v>16</v>
@@ -7153,14 +7335,14 @@
         <v>14</v>
       </c>
       <c r="G28" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H28" s="63">
         <f>E29</f>
         <v>3.5</v>
       </c>
       <c r="I28" s="81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J28" s="63"/>
       <c r="K28" s="82"/>
@@ -7175,14 +7357,14 @@
       <c r="R28" s="17"/>
       <c r="S28" s="84"/>
       <c r="T28" s="27" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="U28" s="93"/>
       <c r="V28" s="23"/>
       <c r="W28" s="84"/>
       <c r="X28" s="21"/>
       <c r="Y28" s="27" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="Z28" s="19"/>
       <c r="AA28" s="21"/>
@@ -7193,7 +7375,7 @@
       <c r="AF28" s="21"/>
       <c r="AG28" s="117"/>
       <c r="AH28" s="27" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="AI28" s="105"/>
       <c r="AJ28" s="105"/>
@@ -7207,7 +7389,7 @@
       <c r="AR28" s="112"/>
       <c r="AS28" s="105"/>
       <c r="AT28" s="27" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="AU28" s="105"/>
       <c r="AV28" s="105"/>
@@ -7220,7 +7402,7 @@
       <c r="BC28" s="105"/>
       <c r="BD28" s="105"/>
       <c r="BE28" s="19" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="BF28" s="105"/>
       <c r="BG28" s="105"/>
@@ -7257,10 +7439,14 @@
       <c r="CL28" s="68"/>
       <c r="CM28" s="68"/>
       <c r="CN28" s="69"/>
-      <c r="CO28" s="239"/>
-      <c r="CP28" s="239"/>
+      <c r="CO28" s="239" t="s">
+        <v>64</v>
+      </c>
+      <c r="CP28" s="239" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="29" spans="1:94" ht="30.5" thickBot="1">
+    <row r="29" spans="1:94" ht="30" thickBot="1">
       <c r="A29" s="217"/>
       <c r="B29" s="40"/>
       <c r="C29" s="100">
@@ -7448,7 +7634,7 @@
       <c r="CO29" s="240"/>
       <c r="CP29" s="240"/>
     </row>
-    <row r="30" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="30" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A30" s="220"/>
       <c r="B30" s="11">
         <v>17</v>
@@ -7461,14 +7647,14 @@
         <v>13</v>
       </c>
       <c r="G30" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H30" s="63">
         <f>E31</f>
         <v>3</v>
       </c>
       <c r="I30" s="81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J30" s="63"/>
       <c r="K30" s="82"/>
@@ -7495,7 +7681,7 @@
       <c r="AD30" s="17"/>
       <c r="AE30" s="84"/>
       <c r="AF30" s="27" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="AG30" s="21"/>
       <c r="AH30" s="27"/>
@@ -7511,7 +7697,7 @@
       <c r="AR30" s="112"/>
       <c r="AS30" s="105"/>
       <c r="AT30" s="27" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="AU30" s="105"/>
       <c r="AV30" s="105"/>
@@ -7526,7 +7712,7 @@
       <c r="BE30" s="105"/>
       <c r="BF30" s="105"/>
       <c r="BG30" s="84" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="BH30" s="21"/>
       <c r="BI30" s="21"/>
@@ -7539,14 +7725,14 @@
       <c r="BP30" s="120"/>
       <c r="BQ30" s="21"/>
       <c r="BR30" s="19" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="BS30" s="21"/>
       <c r="BT30" s="21"/>
       <c r="BU30" s="21"/>
       <c r="BV30" s="21"/>
       <c r="BW30" s="22" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="BX30" s="98"/>
       <c r="BY30" s="63"/>
@@ -7565,10 +7751,14 @@
       <c r="CL30" s="95"/>
       <c r="CM30" s="95"/>
       <c r="CN30" s="99"/>
-      <c r="CO30" s="234"/>
-      <c r="CP30" s="234"/>
+      <c r="CO30" s="234" t="s">
+        <v>64</v>
+      </c>
+      <c r="CP30" s="234" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="31" spans="1:94" ht="30.5" thickBot="1">
+    <row r="31" spans="1:94" ht="30" thickBot="1">
       <c r="A31" s="218"/>
       <c r="B31" s="11"/>
       <c r="C31" s="121">
@@ -7752,7 +7942,7 @@
       <c r="CO31" s="238"/>
       <c r="CP31" s="238"/>
     </row>
-    <row r="32" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="32" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A32" s="216"/>
       <c r="B32" s="80">
         <v>18</v>
@@ -7765,14 +7955,14 @@
         <v>11</v>
       </c>
       <c r="G32" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H32" s="63">
         <f>E33</f>
         <v>2</v>
       </c>
       <c r="I32" s="81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J32" s="63"/>
       <c r="K32" s="82"/>
@@ -7801,7 +7991,7 @@
       <c r="AF32" s="65"/>
       <c r="AG32" s="117"/>
       <c r="AH32" s="27" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="AI32" s="105"/>
       <c r="AJ32" s="105"/>
@@ -7815,7 +8005,7 @@
       <c r="AR32" s="112"/>
       <c r="AS32" s="105"/>
       <c r="AT32" s="27" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="AU32" s="105"/>
       <c r="AV32" s="105"/>
@@ -7839,7 +8029,7 @@
       <c r="BN32" s="24"/>
       <c r="BO32" s="105"/>
       <c r="BP32" s="19" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="BQ32" s="21"/>
       <c r="BR32" s="19"/>
@@ -7865,10 +8055,14 @@
       <c r="CL32" s="68"/>
       <c r="CM32" s="68"/>
       <c r="CN32" s="69"/>
-      <c r="CO32" s="234"/>
-      <c r="CP32" s="234"/>
+      <c r="CO32" s="234" t="s">
+        <v>64</v>
+      </c>
+      <c r="CP32" s="234" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="33" spans="1:94" ht="30.5" thickBot="1">
+    <row r="33" spans="1:94" ht="30" thickBot="1">
       <c r="A33" s="218"/>
       <c r="B33" s="11"/>
       <c r="C33" s="100">
@@ -8044,7 +8238,7 @@
       <c r="CO33" s="238"/>
       <c r="CP33" s="238"/>
     </row>
-    <row r="34" spans="1:94" ht="36" thickTop="1" thickBot="1">
+    <row r="34" spans="1:94" ht="36.75" thickTop="1" thickBot="1">
       <c r="A34" s="219"/>
       <c r="B34" s="80">
         <v>19</v>
@@ -8057,14 +8251,14 @@
         <v>13</v>
       </c>
       <c r="G34" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H34" s="63">
         <f>E35</f>
         <v>3</v>
       </c>
       <c r="I34" s="81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J34" s="63"/>
       <c r="K34" s="82"/>
@@ -8079,14 +8273,14 @@
       <c r="R34" s="17"/>
       <c r="S34" s="84"/>
       <c r="T34" s="27" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="U34" s="93"/>
       <c r="V34" s="23"/>
       <c r="W34" s="84"/>
       <c r="X34" s="21"/>
       <c r="Y34" s="27" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="Z34" s="19"/>
       <c r="AA34" s="21"/>
@@ -8097,7 +8291,7 @@
       <c r="AF34" s="21"/>
       <c r="AG34" s="117"/>
       <c r="AH34" s="27" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="AI34" s="105"/>
       <c r="AJ34" s="105"/>
@@ -8111,7 +8305,7 @@
       <c r="AR34" s="112"/>
       <c r="AS34" s="105"/>
       <c r="AT34" s="27" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="AU34" s="105"/>
       <c r="AV34" s="105"/>
@@ -8159,10 +8353,14 @@
       <c r="CL34" s="95"/>
       <c r="CM34" s="95"/>
       <c r="CN34" s="99"/>
-      <c r="CO34" s="239"/>
-      <c r="CP34" s="239"/>
+      <c r="CO34" s="234" t="s">
+        <v>64</v>
+      </c>
+      <c r="CP34" s="239" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="35" spans="1:94" ht="30.5" thickBot="1">
+    <row r="35" spans="1:94" ht="30" thickBot="1">
       <c r="A35" s="218"/>
       <c r="B35" s="11"/>
       <c r="C35" s="70">
@@ -8346,7 +8544,7 @@
       <c r="CO35" s="240"/>
       <c r="CP35" s="240"/>
     </row>
-    <row r="36" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="36" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A36" s="219"/>
       <c r="B36" s="80">
         <v>20</v>
@@ -8359,14 +8557,14 @@
         <v>7</v>
       </c>
       <c r="G36" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H36" s="17">
         <f>E37</f>
         <v>0</v>
       </c>
       <c r="I36" s="81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J36" s="63"/>
       <c r="K36" s="82"/>
@@ -8395,7 +8593,7 @@
       <c r="AF36" s="65"/>
       <c r="AG36" s="117"/>
       <c r="AH36" s="27" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="AI36" s="105"/>
       <c r="AJ36" s="105"/>
@@ -8409,7 +8607,7 @@
       <c r="AR36" s="112"/>
       <c r="AS36" s="105"/>
       <c r="AT36" s="27" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="AU36" s="105"/>
       <c r="AV36" s="105"/>
@@ -8417,14 +8615,14 @@
       <c r="AX36" s="105"/>
       <c r="AY36" s="105"/>
       <c r="AZ36" s="111" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="BA36" s="105"/>
       <c r="BB36" s="105"/>
       <c r="BC36" s="105"/>
       <c r="BD36" s="105"/>
       <c r="BE36" s="27" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="BF36" s="105"/>
       <c r="BG36" s="105"/>
@@ -8461,10 +8659,14 @@
       <c r="CL36" s="123"/>
       <c r="CM36" s="123"/>
       <c r="CN36" s="124"/>
-      <c r="CO36" s="239"/>
-      <c r="CP36" s="239"/>
+      <c r="CO36" s="234" t="s">
+        <v>64</v>
+      </c>
+      <c r="CP36" s="239" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="37" spans="1:94" ht="30.5" thickBot="1">
+    <row r="37" spans="1:94" ht="30" thickBot="1">
       <c r="A37" s="218"/>
       <c r="B37" s="11"/>
       <c r="C37" s="70">
@@ -8624,7 +8826,7 @@
       <c r="CO37" s="240"/>
       <c r="CP37" s="240"/>
     </row>
-    <row r="38" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="38" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A38" s="219"/>
       <c r="B38" s="80">
         <v>21</v>
@@ -8637,14 +8839,14 @@
         <v>16</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H38" s="17">
         <f>E39</f>
         <v>4.5</v>
       </c>
       <c r="I38" s="81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J38" s="63"/>
       <c r="K38" s="82"/>
@@ -8664,7 +8866,7 @@
       <c r="W38" s="84"/>
       <c r="X38" s="21"/>
       <c r="Y38" s="27" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="Z38" s="19"/>
       <c r="AA38" s="127"/>
@@ -8677,7 +8879,7 @@
       <c r="AH38" s="27"/>
       <c r="AI38" s="105"/>
       <c r="AJ38" s="27" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="AK38" s="21"/>
       <c r="AL38" s="21"/>
@@ -8696,7 +8898,7 @@
       <c r="AY38" s="24"/>
       <c r="AZ38" s="24"/>
       <c r="BA38" s="27" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="BB38" s="27"/>
       <c r="BC38" s="21"/>
@@ -8711,7 +8913,7 @@
       <c r="BL38" s="24"/>
       <c r="BM38" s="105"/>
       <c r="BN38" s="19" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="BO38" s="105"/>
       <c r="BP38" s="105"/>
@@ -8739,10 +8941,14 @@
       <c r="CL38" s="68"/>
       <c r="CM38" s="68"/>
       <c r="CN38" s="69"/>
-      <c r="CO38" s="239"/>
-      <c r="CP38" s="239"/>
+      <c r="CO38" s="239" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP38" s="239" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="39" spans="1:94" ht="30.5" thickBot="1">
+    <row r="39" spans="1:94" ht="30" thickBot="1">
       <c r="A39" s="218"/>
       <c r="B39" s="40"/>
       <c r="C39" s="70">
@@ -8938,7 +9144,7 @@
       <c r="CO39" s="240"/>
       <c r="CP39" s="240"/>
     </row>
-    <row r="40" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="40" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A40" s="216"/>
       <c r="B40" s="80">
         <v>22</v>
@@ -8951,14 +9157,14 @@
         <v>15</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H40" s="17">
         <f>E41</f>
         <v>4</v>
       </c>
       <c r="I40" s="102" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J40" s="17"/>
       <c r="K40" s="49"/>
@@ -8989,7 +9195,7 @@
       <c r="AH40" s="17"/>
       <c r="AI40" s="18"/>
       <c r="AJ40" s="27" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="AK40" s="21"/>
       <c r="AL40" s="21"/>
@@ -9009,7 +9215,7 @@
       <c r="AZ40" s="24"/>
       <c r="BA40" s="21"/>
       <c r="BB40" s="27" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="BC40" s="21"/>
       <c r="BD40" s="21"/>
@@ -9025,7 +9231,7 @@
       <c r="BN40" s="24"/>
       <c r="BO40" s="21"/>
       <c r="BP40" s="27" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="BQ40" s="21"/>
       <c r="BR40" s="21"/>
@@ -9051,10 +9257,14 @@
       <c r="CL40" s="95"/>
       <c r="CM40" s="95"/>
       <c r="CN40" s="99"/>
-      <c r="CO40" s="234"/>
-      <c r="CP40" s="234"/>
+      <c r="CO40" s="234" t="s">
+        <v>97</v>
+      </c>
+      <c r="CP40" s="234" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="41" spans="1:94" ht="30.5" thickBot="1">
+    <row r="41" spans="1:94" ht="30" thickBot="1">
       <c r="A41" s="218"/>
       <c r="B41" s="40"/>
       <c r="C41" s="41">
@@ -9246,7 +9456,7 @@
       <c r="CO41" s="238"/>
       <c r="CP41" s="238"/>
     </row>
-    <row r="42" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="42" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A42" s="216"/>
       <c r="B42" s="80">
         <v>23</v>
@@ -9259,7 +9469,7 @@
         <v>10</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H42" s="17">
         <f>E43</f>
@@ -9295,7 +9505,7 @@
       <c r="AJ42" s="65"/>
       <c r="AK42" s="18"/>
       <c r="AL42" s="27" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="AM42" s="21"/>
       <c r="AN42" s="21"/>
@@ -9309,7 +9519,7 @@
       <c r="AV42" s="24"/>
       <c r="AW42" s="21"/>
       <c r="AX42" s="27" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="AY42" s="21"/>
       <c r="AZ42" s="127"/>
@@ -9332,7 +9542,7 @@
       <c r="BQ42" s="24"/>
       <c r="BR42" s="24"/>
       <c r="BS42" s="19" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="BT42" s="21"/>
       <c r="BU42" s="22"/>
@@ -9355,10 +9565,14 @@
       <c r="CL42" s="133"/>
       <c r="CM42" s="133"/>
       <c r="CN42" s="99"/>
-      <c r="CO42" s="234"/>
-      <c r="CP42" s="234"/>
+      <c r="CO42" s="234" t="s">
+        <v>101</v>
+      </c>
+      <c r="CP42" s="234" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="43" spans="1:94" ht="30.5" thickBot="1">
+    <row r="43" spans="1:94" ht="30" thickBot="1">
       <c r="A43" s="221"/>
       <c r="B43" s="11"/>
       <c r="C43" s="41">
@@ -9530,7 +9744,7 @@
       <c r="CO43" s="238"/>
       <c r="CP43" s="238"/>
     </row>
-    <row r="44" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="44" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A44" s="218"/>
       <c r="B44" s="80">
         <v>24</v>
@@ -9543,7 +9757,7 @@
         <v>11</v>
       </c>
       <c r="G44" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H44" s="63">
         <f>E45</f>
@@ -9579,7 +9793,7 @@
       <c r="AJ44" s="65"/>
       <c r="AK44" s="18"/>
       <c r="AL44" s="27" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="AM44" s="21"/>
       <c r="AN44" s="21"/>
@@ -9593,7 +9807,7 @@
       <c r="AV44" s="24"/>
       <c r="AW44" s="21"/>
       <c r="AX44" s="27" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="AY44" s="21"/>
       <c r="AZ44" s="127"/>
@@ -9613,13 +9827,13 @@
       <c r="BN44" s="24"/>
       <c r="BO44" s="105"/>
       <c r="BP44" s="19" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="BQ44" s="105"/>
       <c r="BR44" s="105"/>
       <c r="BS44" s="111"/>
       <c r="BT44" s="27" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="BU44" s="21"/>
       <c r="BV44" s="21"/>
@@ -9641,10 +9855,14 @@
       <c r="CL44" s="95"/>
       <c r="CM44" s="95"/>
       <c r="CN44" s="99"/>
-      <c r="CO44" s="239"/>
-      <c r="CP44" s="239"/>
+      <c r="CO44" s="239" t="s">
+        <v>21</v>
+      </c>
+      <c r="CP44" s="239" t="s">
+        <v>106</v>
+      </c>
     </row>
-    <row r="45" spans="1:94" ht="30.5" thickBot="1">
+    <row r="45" spans="1:94" ht="30" thickBot="1">
       <c r="A45" s="217"/>
       <c r="B45" s="11"/>
       <c r="C45" s="70">
@@ -9820,7 +10038,7 @@
       <c r="CO45" s="240"/>
       <c r="CP45" s="240"/>
     </row>
-    <row r="46" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="46" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A46" s="216"/>
       <c r="B46" s="80">
         <v>25</v>
@@ -9833,14 +10051,14 @@
         <v>10</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H46" s="17">
         <f>E47</f>
         <v>1.5</v>
       </c>
       <c r="I46" s="102" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J46" s="63"/>
       <c r="K46" s="82"/>
@@ -9875,7 +10093,7 @@
       <c r="AL46" s="63"/>
       <c r="AM46" s="18"/>
       <c r="AN46" s="27" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="AO46" s="21"/>
       <c r="AP46" s="21"/>
@@ -9893,7 +10111,7 @@
       <c r="BB46" s="106"/>
       <c r="BC46" s="21"/>
       <c r="BD46" s="27" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="BE46" s="21"/>
       <c r="BF46" s="21"/>
@@ -9906,11 +10124,11 @@
       <c r="BM46" s="24"/>
       <c r="BN46" s="24"/>
       <c r="BO46" s="27" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="BP46" s="27"/>
       <c r="BQ46" s="27" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="BR46" s="21"/>
       <c r="BS46" s="21"/>
@@ -9935,10 +10153,14 @@
       <c r="CL46" s="68"/>
       <c r="CM46" s="68"/>
       <c r="CN46" s="69"/>
-      <c r="CO46" s="239"/>
-      <c r="CP46" s="239"/>
+      <c r="CO46" s="239" t="s">
+        <v>110</v>
+      </c>
+      <c r="CP46" s="239" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="47" spans="1:94" ht="30.5" thickBot="1">
+    <row r="47" spans="1:94" ht="30" thickBot="1">
       <c r="A47" s="217"/>
       <c r="B47" s="40"/>
       <c r="C47" s="134">
@@ -10110,7 +10332,7 @@
       <c r="CO47" s="240"/>
       <c r="CP47" s="240"/>
     </row>
-    <row r="48" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="48" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A48" s="222"/>
       <c r="B48" s="80">
         <v>26</v>
@@ -10123,14 +10345,14 @@
         <v>12</v>
       </c>
       <c r="G48" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H48" s="63">
         <f>E49</f>
         <v>2.5</v>
       </c>
       <c r="I48" s="102" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J48" s="17"/>
       <c r="K48" s="49"/>
@@ -10165,7 +10387,7 @@
       <c r="AL48" s="63"/>
       <c r="AM48" s="18"/>
       <c r="AN48" s="27" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="AO48" s="21"/>
       <c r="AP48" s="21"/>
@@ -10181,7 +10403,7 @@
       <c r="AZ48" s="24"/>
       <c r="BA48" s="30"/>
       <c r="BB48" s="27" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="BC48" s="21"/>
       <c r="BD48" s="21"/>
@@ -10221,10 +10443,14 @@
       <c r="CL48" s="68"/>
       <c r="CM48" s="68"/>
       <c r="CN48" s="69"/>
-      <c r="CO48" s="234"/>
-      <c r="CP48" s="234"/>
+      <c r="CO48" s="234" t="s">
+        <v>114</v>
+      </c>
+      <c r="CP48" s="239" t="s">
+        <v>115</v>
+      </c>
     </row>
-    <row r="49" spans="1:94" ht="30.5" thickBot="1">
+    <row r="49" spans="1:94" ht="30" thickBot="1">
       <c r="A49" s="218"/>
       <c r="B49" s="40"/>
       <c r="C49" s="70">
@@ -10404,7 +10630,7 @@
       <c r="CO49" s="238"/>
       <c r="CP49" s="238"/>
     </row>
-    <row r="50" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="50" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A50" s="219"/>
       <c r="B50" s="80">
         <v>27</v>
@@ -10417,14 +10643,14 @@
         <v>10</v>
       </c>
       <c r="G50" s="16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H50" s="17">
         <f>E51</f>
         <v>1.5</v>
       </c>
       <c r="I50" s="81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J50" s="63"/>
       <c r="K50" s="82"/>
@@ -10459,7 +10685,7 @@
       <c r="AL50" s="17"/>
       <c r="AM50" s="18"/>
       <c r="AN50" s="27" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="AO50" s="21"/>
       <c r="AP50" s="21"/>
@@ -10475,7 +10701,7 @@
       <c r="AZ50" s="24"/>
       <c r="BA50" s="30"/>
       <c r="BB50" s="27" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="BC50" s="21"/>
       <c r="BD50" s="21"/>
@@ -10515,10 +10741,14 @@
       <c r="CL50" s="68"/>
       <c r="CM50" s="68"/>
       <c r="CN50" s="69"/>
-      <c r="CO50" s="234"/>
-      <c r="CP50" s="234"/>
+      <c r="CO50" s="234" t="s">
+        <v>114</v>
+      </c>
+      <c r="CP50" s="239" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="51" spans="1:94" ht="30.5" thickBot="1">
+    <row r="51" spans="1:94" ht="30" thickBot="1">
       <c r="A51" s="217"/>
       <c r="B51" s="80"/>
       <c r="C51" s="70">
@@ -10690,7 +10920,7 @@
       <c r="CO51" s="238"/>
       <c r="CP51" s="238"/>
     </row>
-    <row r="52" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="52" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A52" s="218"/>
       <c r="B52" s="80">
         <v>28</v>
@@ -10703,7 +10933,7 @@
         <v>10</v>
       </c>
       <c r="G52" s="16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H52" s="17">
         <f>E53</f>
@@ -10743,7 +10973,7 @@
       <c r="AN52" s="49"/>
       <c r="AO52" s="18"/>
       <c r="AP52" s="27" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="AQ52" s="21"/>
       <c r="AR52" s="21"/>
@@ -10755,7 +10985,7 @@
       <c r="AX52" s="27"/>
       <c r="AY52" s="18"/>
       <c r="AZ52" s="19" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="BA52" s="20"/>
       <c r="BB52" s="131"/>
@@ -10772,21 +11002,21 @@
       <c r="BM52" s="24"/>
       <c r="BN52" s="24"/>
       <c r="BO52" s="136" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="BP52" s="27"/>
       <c r="BQ52" s="21"/>
       <c r="BR52" s="21"/>
       <c r="BS52" s="111"/>
       <c r="BT52" s="27" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="BU52" s="21"/>
       <c r="BV52" s="21"/>
       <c r="BW52" s="21"/>
       <c r="BX52" s="21"/>
       <c r="BY52" s="137" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="BZ52" s="98"/>
       <c r="CA52" s="17"/>
@@ -10803,10 +11033,14 @@
       <c r="CL52" s="123"/>
       <c r="CM52" s="123"/>
       <c r="CN52" s="69"/>
-      <c r="CO52" s="239"/>
-      <c r="CP52" s="239"/>
+      <c r="CO52" s="239" t="s">
+        <v>21</v>
+      </c>
+      <c r="CP52" s="239" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="53" spans="1:94" ht="30.5" thickBot="1">
+    <row r="53" spans="1:94" ht="30" thickBot="1">
       <c r="A53" s="221"/>
       <c r="B53" s="11"/>
       <c r="C53" s="41">
@@ -10978,7 +11212,7 @@
       <c r="CO53" s="240"/>
       <c r="CP53" s="240"/>
     </row>
-    <row r="54" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="54" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A54" s="219"/>
       <c r="B54" s="80">
         <v>29</v>
@@ -10991,7 +11225,7 @@
         <v>12</v>
       </c>
       <c r="G54" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H54" s="17">
         <f>E55</f>
@@ -11030,7 +11264,7 @@
       <c r="AM54" s="17"/>
       <c r="AN54" s="63"/>
       <c r="AO54" s="111" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="AP54" s="27"/>
       <c r="AQ54" s="27"/>
@@ -11040,7 +11274,7 @@
       <c r="AU54" s="18"/>
       <c r="AV54" s="21"/>
       <c r="AW54" s="27" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="AX54" s="21"/>
       <c r="AY54" s="21"/>
@@ -11051,14 +11285,14 @@
       <c r="BD54" s="21"/>
       <c r="BE54" s="21"/>
       <c r="BF54" s="111" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="BG54" s="21"/>
       <c r="BH54" s="21"/>
       <c r="BI54" s="21"/>
       <c r="BJ54" s="21"/>
       <c r="BK54" s="111" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="BL54" s="21"/>
       <c r="BM54" s="24"/>
@@ -11067,7 +11301,7 @@
       <c r="BP54" s="135"/>
       <c r="BQ54" s="21"/>
       <c r="BR54" s="27" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="BS54" s="21"/>
       <c r="BT54" s="21"/>
@@ -11091,10 +11325,14 @@
       <c r="CL54" s="68"/>
       <c r="CM54" s="68"/>
       <c r="CN54" s="69"/>
-      <c r="CO54" s="239"/>
-      <c r="CP54" s="239"/>
+      <c r="CO54" s="239" t="s">
+        <v>126</v>
+      </c>
+      <c r="CP54" s="239" t="s">
+        <v>127</v>
+      </c>
     </row>
-    <row r="55" spans="1:94" ht="30.5" thickBot="1">
+    <row r="55" spans="1:94" ht="30" thickBot="1">
       <c r="A55" s="217"/>
       <c r="B55" s="11"/>
       <c r="C55" s="70">
@@ -11274,7 +11512,7 @@
       <c r="CO55" s="240"/>
       <c r="CP55" s="240"/>
     </row>
-    <row r="56" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="56" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A56" s="219"/>
       <c r="B56" s="80">
         <v>30</v>
@@ -11287,14 +11525,14 @@
         <v>11</v>
       </c>
       <c r="G56" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H56" s="17">
         <f>E57</f>
         <v>2</v>
       </c>
       <c r="I56" s="81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J56" s="63"/>
       <c r="K56" s="82"/>
@@ -11334,7 +11572,7 @@
       <c r="AQ56" s="18"/>
       <c r="AR56" s="21"/>
       <c r="AS56" s="27" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="AT56" s="21"/>
       <c r="AU56" s="21"/>
@@ -11355,7 +11593,7 @@
       <c r="BJ56" s="135"/>
       <c r="BK56" s="21"/>
       <c r="BL56" s="27" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
       <c r="BM56" s="21"/>
       <c r="BN56" s="21"/>
@@ -11371,14 +11609,14 @@
       <c r="BX56" s="21"/>
       <c r="BY56" s="21"/>
       <c r="BZ56" s="111" t="s">
-        <v>89</v>
+        <v>130</v>
       </c>
       <c r="CA56" s="21"/>
       <c r="CB56" s="21"/>
       <c r="CC56" s="21"/>
       <c r="CD56" s="98"/>
       <c r="CE56" s="92" t="s">
-        <v>90</v>
+        <v>131</v>
       </c>
       <c r="CF56" s="65"/>
       <c r="CG56" s="66"/>
@@ -11389,10 +11627,14 @@
       <c r="CL56" s="95"/>
       <c r="CM56" s="95"/>
       <c r="CN56" s="99"/>
-      <c r="CO56" s="234"/>
-      <c r="CP56" s="234"/>
+      <c r="CO56" s="234" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP56" s="234" t="s">
+        <v>132</v>
+      </c>
     </row>
-    <row r="57" spans="1:94" ht="30.5" thickBot="1">
+    <row r="57" spans="1:94" ht="30" thickBot="1">
       <c r="A57" s="217"/>
       <c r="B57" s="139"/>
       <c r="C57" s="70">
@@ -11568,7 +11810,7 @@
       <c r="CO57" s="238"/>
       <c r="CP57" s="238"/>
     </row>
-    <row r="58" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="58" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A58" s="219"/>
       <c r="B58" s="80">
         <v>31</v>
@@ -11581,7 +11823,7 @@
         <v>7</v>
       </c>
       <c r="G58" s="16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H58" s="17">
         <f>E59</f>
@@ -11600,7 +11842,7 @@
       <c r="S58" s="84"/>
       <c r="T58" s="27"/>
       <c r="U58" s="27" t="s">
-        <v>91</v>
+        <v>133</v>
       </c>
       <c r="V58" s="21"/>
       <c r="W58" s="19"/>
@@ -11614,7 +11856,7 @@
       <c r="AE58" s="21"/>
       <c r="AF58" s="21"/>
       <c r="AG58" s="111" t="s">
-        <v>92</v>
+        <v>134</v>
       </c>
       <c r="AH58" s="27"/>
       <c r="AI58" s="105"/>
@@ -11625,7 +11867,7 @@
       <c r="AN58" s="135"/>
       <c r="AO58" s="21"/>
       <c r="AP58" s="27" t="s">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="AQ58" s="21"/>
       <c r="AR58" s="21"/>
@@ -11677,10 +11919,14 @@
       <c r="CL58" s="133"/>
       <c r="CM58" s="133"/>
       <c r="CN58" s="99"/>
-      <c r="CO58" s="234"/>
-      <c r="CP58" s="234"/>
+      <c r="CO58" s="234" t="s">
+        <v>21</v>
+      </c>
+      <c r="CP58" s="234" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="59" spans="1:94" ht="30.5" thickBot="1">
+    <row r="59" spans="1:94" ht="30" thickBot="1">
       <c r="A59" s="218"/>
       <c r="B59" s="40"/>
       <c r="C59" s="70">
@@ -11840,7 +12086,7 @@
       <c r="CO59" s="238"/>
       <c r="CP59" s="238"/>
     </row>
-    <row r="60" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="60" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A60" s="219"/>
       <c r="B60" s="80">
         <v>32</v>
@@ -11853,7 +12099,7 @@
         <v>12</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H60" s="17">
         <f>E61</f>
@@ -11872,7 +12118,7 @@
       <c r="S60" s="84"/>
       <c r="T60" s="23"/>
       <c r="U60" s="27" t="s">
-        <v>94</v>
+        <v>137</v>
       </c>
       <c r="V60" s="21"/>
       <c r="W60" s="21"/>
@@ -11903,7 +12149,7 @@
       <c r="AV60" s="19"/>
       <c r="AW60" s="20"/>
       <c r="AX60" s="29" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="AY60" s="22"/>
       <c r="AZ60" s="23"/>
@@ -11911,12 +12157,12 @@
       <c r="BB60" s="21"/>
       <c r="BC60" s="18"/>
       <c r="BD60" s="29" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="BE60" s="20"/>
       <c r="BF60" s="21"/>
       <c r="BG60" s="30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="BH60" s="23"/>
       <c r="BI60" s="64"/>
@@ -11951,10 +12197,14 @@
       <c r="CL60" s="133"/>
       <c r="CM60" s="133"/>
       <c r="CN60" s="99"/>
-      <c r="CO60" s="234"/>
-      <c r="CP60" s="234"/>
+      <c r="CO60" s="234" t="s">
+        <v>138</v>
+      </c>
+      <c r="CP60" s="234" t="s">
+        <v>139</v>
+      </c>
     </row>
-    <row r="61" spans="1:94" ht="30.5" thickBot="1">
+    <row r="61" spans="1:94" ht="30" thickBot="1">
       <c r="A61" s="217"/>
       <c r="B61" s="40"/>
       <c r="C61" s="41">
@@ -12134,7 +12384,7 @@
       <c r="CO61" s="238"/>
       <c r="CP61" s="238"/>
     </row>
-    <row r="62" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="62" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A62" s="216"/>
       <c r="B62" s="11">
         <v>33</v>
@@ -12147,14 +12397,14 @@
         <v>10</v>
       </c>
       <c r="G62" s="16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H62" s="17">
         <f>E63</f>
         <v>1.5</v>
       </c>
       <c r="I62" s="81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J62" s="17"/>
       <c r="K62" s="82"/>
@@ -12198,7 +12448,7 @@
       <c r="AU62" s="18"/>
       <c r="AV62" s="21"/>
       <c r="AW62" s="27" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="AX62" s="27"/>
       <c r="AY62" s="21"/>
@@ -12206,7 +12456,7 @@
       <c r="BA62" s="30"/>
       <c r="BB62" s="21"/>
       <c r="BC62" s="111" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="BD62" s="21"/>
       <c r="BE62" s="127"/>
@@ -12221,7 +12471,7 @@
       <c r="BN62" s="24"/>
       <c r="BO62" s="127"/>
       <c r="BP62" s="27" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
       <c r="BQ62" s="127"/>
       <c r="BR62" s="127"/>
@@ -12247,10 +12497,14 @@
       <c r="CL62" s="123"/>
       <c r="CM62" s="123"/>
       <c r="CN62" s="69"/>
-      <c r="CO62" s="234"/>
-      <c r="CP62" s="234"/>
+      <c r="CO62" s="234" t="s">
+        <v>142</v>
+      </c>
+      <c r="CP62" s="234" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="63" spans="1:94" ht="30.5" thickBot="1">
+    <row r="63" spans="1:94" ht="30" thickBot="1">
       <c r="A63" s="221"/>
       <c r="B63" s="40"/>
       <c r="C63" s="41">
@@ -12422,7 +12676,7 @@
       <c r="CO63" s="238"/>
       <c r="CP63" s="238"/>
     </row>
-    <row r="64" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="64" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A64" s="223"/>
       <c r="B64" s="11">
         <v>34</v>
@@ -12435,7 +12689,7 @@
         <v>8</v>
       </c>
       <c r="G64" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H64" s="63">
         <f>E65</f>
@@ -12483,7 +12737,7 @@
       <c r="AV64" s="19"/>
       <c r="AW64" s="20"/>
       <c r="AX64" s="29" t="s">
-        <v>97</v>
+        <v>144</v>
       </c>
       <c r="AY64" s="22"/>
       <c r="AZ64" s="23"/>
@@ -12491,12 +12745,12 @@
       <c r="BB64" s="21"/>
       <c r="BC64" s="18"/>
       <c r="BD64" s="29" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="BE64" s="20"/>
       <c r="BF64" s="21"/>
       <c r="BG64" s="30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="BH64" s="21"/>
       <c r="BI64" s="21"/>
@@ -12508,7 +12762,7 @@
       <c r="BO64" s="27"/>
       <c r="BP64" s="27"/>
       <c r="BQ64" s="27" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="BR64" s="21"/>
       <c r="BS64" s="21"/>
@@ -12533,10 +12787,14 @@
       <c r="CL64" s="95"/>
       <c r="CM64" s="95"/>
       <c r="CN64" s="99"/>
-      <c r="CO64" s="234"/>
-      <c r="CP64" s="234"/>
+      <c r="CO64" s="234" t="s">
+        <v>21</v>
+      </c>
+      <c r="CP64" s="234" t="s">
+        <v>145</v>
+      </c>
     </row>
-    <row r="65" spans="1:94" ht="30.5" thickBot="1">
+    <row r="65" spans="1:94" ht="30" thickBot="1">
       <c r="A65" s="224"/>
       <c r="B65" s="11"/>
       <c r="C65" s="100">
@@ -12700,7 +12958,7 @@
       <c r="CO65" s="238"/>
       <c r="CP65" s="238"/>
     </row>
-    <row r="66" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="66" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A66" s="219"/>
       <c r="B66" s="80">
         <v>35</v>
@@ -12713,14 +12971,14 @@
         <v>12</v>
       </c>
       <c r="G66" s="62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H66" s="17">
         <f>E67</f>
         <v>2.5</v>
       </c>
       <c r="I66" s="81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J66" s="63"/>
       <c r="K66" s="82"/>
@@ -12757,7 +13015,7 @@
       <c r="AN66" s="63"/>
       <c r="AO66" s="18"/>
       <c r="AP66" s="27" t="s">
-        <v>98</v>
+        <v>146</v>
       </c>
       <c r="AQ66" s="21"/>
       <c r="AR66" s="21"/>
@@ -12769,7 +13027,7 @@
       <c r="AX66" s="98"/>
       <c r="AY66" s="18"/>
       <c r="AZ66" s="19" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="BA66" s="20"/>
       <c r="BB66" s="131"/>
@@ -12786,7 +13044,7 @@
       <c r="BM66" s="24"/>
       <c r="BN66" s="24"/>
       <c r="BO66" s="19" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="BP66" s="19"/>
       <c r="BQ66" s="21"/>
@@ -12800,13 +13058,13 @@
       <c r="BY66" s="21"/>
       <c r="BZ66" s="98"/>
       <c r="CA66" s="27" t="s">
-        <v>89</v>
+        <v>130</v>
       </c>
       <c r="CB66" s="21"/>
       <c r="CC66" s="21"/>
       <c r="CD66" s="98"/>
       <c r="CE66" s="92" t="s">
-        <v>90</v>
+        <v>131</v>
       </c>
       <c r="CF66" s="140"/>
       <c r="CG66" s="66"/>
@@ -12817,10 +13075,14 @@
       <c r="CL66" s="133"/>
       <c r="CM66" s="133"/>
       <c r="CN66" s="99"/>
-      <c r="CO66" s="234"/>
-      <c r="CP66" s="234"/>
+      <c r="CO66" s="234" t="s">
+        <v>21</v>
+      </c>
+      <c r="CP66" s="234" t="s">
+        <v>127</v>
+      </c>
     </row>
-    <row r="67" spans="1:94" ht="30.5" thickBot="1">
+    <row r="67" spans="1:94" ht="30" thickBot="1">
       <c r="A67" s="217"/>
       <c r="B67" s="141"/>
       <c r="C67" s="142">
@@ -13000,7 +13262,7 @@
       <c r="CO67" s="238"/>
       <c r="CP67" s="238"/>
     </row>
-    <row r="68" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="68" spans="1:94" ht="30.4" thickTop="1" thickBot="1">
       <c r="A68" s="225"/>
       <c r="B68" s="144">
         <v>36</v>
@@ -13013,7 +13275,7 @@
         <v>9</v>
       </c>
       <c r="G68" s="16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H68" s="17">
         <f>E69</f>
@@ -13054,14 +13316,14 @@
       <c r="AO68" s="108"/>
       <c r="AP68" s="49"/>
       <c r="AQ68" s="145" t="s">
-        <v>99</v>
+        <v>147</v>
       </c>
       <c r="AR68" s="23"/>
       <c r="AS68" s="20"/>
       <c r="AT68" s="21"/>
       <c r="AU68" s="18"/>
       <c r="AV68" s="29" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="AW68" s="20"/>
       <c r="AX68" s="21"/>
@@ -13070,12 +13332,12 @@
       <c r="BA68" s="21"/>
       <c r="BB68" s="21"/>
       <c r="BC68" s="146" t="s">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="BD68" s="20"/>
       <c r="BE68" s="21"/>
       <c r="BF68" s="30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="BG68" s="30"/>
       <c r="BH68" s="23"/>
@@ -13088,7 +13350,7 @@
       <c r="BO68" s="27"/>
       <c r="BP68" s="27"/>
       <c r="BQ68" s="27" t="s">
-        <v>101</v>
+        <v>149</v>
       </c>
       <c r="BR68" s="21"/>
       <c r="BS68" s="21"/>
@@ -13113,10 +13375,14 @@
       <c r="CL68" s="133"/>
       <c r="CM68" s="133"/>
       <c r="CN68" s="99"/>
-      <c r="CO68" s="239"/>
-      <c r="CP68" s="239"/>
+      <c r="CO68" s="239" t="s">
+        <v>21</v>
+      </c>
+      <c r="CP68" s="239" t="s">
+        <v>150</v>
+      </c>
     </row>
-    <row r="69" spans="1:94" ht="30.5" thickBot="1">
+    <row r="69" spans="1:94" ht="30" thickBot="1">
       <c r="A69" s="226"/>
       <c r="B69" s="141"/>
       <c r="C69" s="41">
@@ -13284,7 +13550,7 @@
       <c r="CO69" s="240"/>
       <c r="CP69" s="240"/>
     </row>
-    <row r="70" spans="1:94" ht="30.5" thickTop="1">
+    <row r="70" spans="1:94" ht="30" thickTop="1">
       <c r="A70" s="227"/>
       <c r="B70" s="147">
         <v>36</v>
@@ -13382,7 +13648,7 @@
       <c r="CO70" s="239"/>
       <c r="CP70" s="239"/>
     </row>
-    <row r="71" spans="1:94" ht="30.5" thickBot="1">
+    <row r="71" spans="1:94" ht="30" thickBot="1">
       <c r="A71" s="221"/>
       <c r="B71" s="144"/>
       <c r="C71" s="41"/>
@@ -13866,136 +14132,136 @@
       <c r="A76" s="215"/>
       <c r="B76" s="160"/>
       <c r="C76" s="2" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="161"/>
       <c r="F76" s="3"/>
       <c r="G76" s="4"/>
-      <c r="H76" s="268">
+      <c r="H76" s="244">
         <v>4</v>
       </c>
-      <c r="I76" s="268"/>
+      <c r="I76" s="244"/>
       <c r="J76" s="131"/>
       <c r="K76" s="131"/>
-      <c r="L76" s="268">
+      <c r="L76" s="244">
         <v>5</v>
       </c>
-      <c r="M76" s="268"/>
+      <c r="M76" s="244"/>
       <c r="N76" s="3"/>
       <c r="O76" s="3"/>
-      <c r="P76" s="268">
+      <c r="P76" s="244">
         <v>6</v>
       </c>
-      <c r="Q76" s="268"/>
+      <c r="Q76" s="244"/>
       <c r="R76" s="8"/>
       <c r="S76" s="8"/>
-      <c r="T76" s="268">
+      <c r="T76" s="244">
         <v>7</v>
       </c>
-      <c r="U76" s="268"/>
+      <c r="U76" s="244"/>
       <c r="V76" s="8"/>
       <c r="W76" s="8"/>
-      <c r="X76" s="268">
+      <c r="X76" s="244">
         <v>8</v>
       </c>
-      <c r="Y76" s="268"/>
+      <c r="Y76" s="244"/>
       <c r="Z76" s="8"/>
       <c r="AA76" s="8"/>
-      <c r="AB76" s="268">
+      <c r="AB76" s="244">
         <v>9</v>
       </c>
-      <c r="AC76" s="268"/>
+      <c r="AC76" s="244"/>
       <c r="AD76" s="8"/>
       <c r="AE76" s="8"/>
-      <c r="AF76" s="268">
+      <c r="AF76" s="244">
         <v>10</v>
       </c>
-      <c r="AG76" s="268"/>
+      <c r="AG76" s="244"/>
       <c r="AH76" s="8"/>
       <c r="AI76" s="8"/>
-      <c r="AJ76" s="268">
+      <c r="AJ76" s="244">
         <v>11</v>
       </c>
-      <c r="AK76" s="268"/>
+      <c r="AK76" s="244"/>
       <c r="AL76" s="8"/>
       <c r="AM76" s="8"/>
-      <c r="AN76" s="268">
+      <c r="AN76" s="244">
         <v>12</v>
       </c>
-      <c r="AO76" s="268"/>
+      <c r="AO76" s="244"/>
       <c r="AP76" s="8"/>
       <c r="AQ76" s="8"/>
-      <c r="AR76" s="268">
+      <c r="AR76" s="244">
         <v>13</v>
       </c>
-      <c r="AS76" s="268"/>
+      <c r="AS76" s="244"/>
       <c r="AT76" s="8"/>
       <c r="AU76" s="8"/>
-      <c r="AV76" s="268">
+      <c r="AV76" s="244">
         <v>14</v>
       </c>
-      <c r="AW76" s="268"/>
+      <c r="AW76" s="244"/>
       <c r="AX76" s="8"/>
       <c r="AY76" s="8"/>
-      <c r="AZ76" s="268">
+      <c r="AZ76" s="244">
         <v>15</v>
       </c>
-      <c r="BA76" s="268"/>
+      <c r="BA76" s="244"/>
       <c r="BB76" s="8"/>
       <c r="BC76" s="8"/>
-      <c r="BD76" s="268">
+      <c r="BD76" s="244">
         <v>16</v>
       </c>
-      <c r="BE76" s="268"/>
+      <c r="BE76" s="244"/>
       <c r="BF76" s="8"/>
       <c r="BG76" s="8"/>
-      <c r="BH76" s="268">
+      <c r="BH76" s="244">
         <v>17</v>
       </c>
-      <c r="BI76" s="268"/>
+      <c r="BI76" s="244"/>
       <c r="BJ76" s="8"/>
       <c r="BK76" s="8"/>
-      <c r="BL76" s="268">
+      <c r="BL76" s="244">
         <v>18</v>
       </c>
-      <c r="BM76" s="268"/>
+      <c r="BM76" s="244"/>
       <c r="BN76" s="8"/>
       <c r="BO76" s="8"/>
-      <c r="BP76" s="268">
+      <c r="BP76" s="244">
         <v>19</v>
       </c>
-      <c r="BQ76" s="268"/>
+      <c r="BQ76" s="244"/>
       <c r="BR76" s="8"/>
       <c r="BS76" s="8"/>
-      <c r="BT76" s="268">
+      <c r="BT76" s="244">
         <v>20</v>
       </c>
-      <c r="BU76" s="268"/>
+      <c r="BU76" s="244"/>
       <c r="BV76" s="8"/>
       <c r="BW76" s="8"/>
-      <c r="BX76" s="268">
+      <c r="BX76" s="244">
         <v>21</v>
       </c>
-      <c r="BY76" s="268"/>
+      <c r="BY76" s="244"/>
       <c r="BZ76" s="162"/>
       <c r="CA76" s="162"/>
-      <c r="CB76" s="268">
+      <c r="CB76" s="244">
         <v>22</v>
       </c>
-      <c r="CC76" s="268"/>
+      <c r="CC76" s="244"/>
       <c r="CD76" s="162"/>
       <c r="CE76" s="8"/>
-      <c r="CF76" s="268">
+      <c r="CF76" s="244">
         <v>23</v>
       </c>
-      <c r="CG76" s="268"/>
+      <c r="CG76" s="244"/>
       <c r="CH76" s="8"/>
       <c r="CI76" s="8"/>
-      <c r="CJ76" s="268">
+      <c r="CJ76" s="244">
         <v>24</v>
       </c>
-      <c r="CK76" s="268"/>
+      <c r="CK76" s="244"/>
       <c r="CL76" s="8"/>
       <c r="CM76" s="8"/>
       <c r="CN76" s="8"/>
@@ -14007,7 +14273,7 @@
         <v>299.5</v>
       </c>
       <c r="C77" s="164" t="s">
-        <v>103</v>
+        <v>152</v>
       </c>
       <c r="D77" s="165">
         <f>SUM(B77)</f>
@@ -14016,11 +14282,11 @@
       <c r="E77" s="166">
         <v>3</v>
       </c>
-      <c r="F77" s="269">
+      <c r="F77" s="246">
         <f>SUM(D77,E78)</f>
         <v>299.5</v>
       </c>
-      <c r="G77" s="270"/>
+      <c r="G77" s="247"/>
       <c r="H77" s="167"/>
       <c r="I77" s="123"/>
       <c r="J77" s="123"/>
@@ -14109,7 +14375,7 @@
     </row>
     <row r="78" spans="1:94" ht="30" thickBot="1">
       <c r="A78" s="230" t="s">
-        <v>104</v>
+        <v>153</v>
       </c>
       <c r="B78" s="173">
         <f>SUM(E2:E75)</f>
@@ -14118,8 +14384,8 @@
       <c r="C78" s="174"/>
       <c r="D78" s="175"/>
       <c r="E78" s="176"/>
-      <c r="F78" s="256"/>
-      <c r="G78" s="257"/>
+      <c r="F78" s="248"/>
+      <c r="G78" s="249"/>
       <c r="H78" s="177"/>
       <c r="I78" s="123"/>
       <c r="J78" s="123"/>
@@ -14206,7 +14472,7 @@
       <c r="CM78" s="68"/>
       <c r="CN78" s="68"/>
     </row>
-    <row r="79" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="79" spans="1:94" ht="30.75" thickTop="1" thickBot="1">
       <c r="A79" s="231">
         <f>SUM(A80:B80)</f>
         <v>34</v>
@@ -14216,15 +14482,15 @@
         <v>238</v>
       </c>
       <c r="C79" s="179" t="s">
-        <v>105</v>
+        <v>154</v>
       </c>
       <c r="D79" s="180"/>
       <c r="E79" s="181"/>
-      <c r="F79" s="261">
+      <c r="F79" s="250">
         <f>SUM(F77-B79)</f>
         <v>61.5</v>
       </c>
-      <c r="G79" s="262"/>
+      <c r="G79" s="251"/>
       <c r="H79" s="182"/>
       <c r="I79" s="123"/>
       <c r="J79" s="123"/>
@@ -14232,7 +14498,7 @@
       <c r="L79" s="123"/>
       <c r="M79" s="123"/>
       <c r="N79" s="183" t="s">
-        <v>106</v>
+        <v>155</v>
       </c>
       <c r="O79" s="172"/>
       <c r="P79" s="172"/>
@@ -14242,15 +14508,15 @@
       <c r="T79" s="123"/>
       <c r="U79" s="123"/>
       <c r="V79" s="184" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="W79" s="123"/>
-      <c r="X79" s="258">
+      <c r="X79" s="252">
         <f>F77</f>
         <v>299.5</v>
       </c>
-      <c r="Y79" s="259"/>
-      <c r="Z79" s="260"/>
+      <c r="Y79" s="253"/>
+      <c r="Z79" s="254"/>
       <c r="AA79" s="172"/>
       <c r="AB79" s="172"/>
       <c r="AC79" s="185"/>
@@ -14318,25 +14584,25 @@
       <c r="CM79" s="68"/>
       <c r="CN79" s="68"/>
     </row>
-    <row r="80" spans="1:94" ht="31" thickTop="1" thickBot="1">
+    <row r="80" spans="1:94" ht="30.75" thickTop="1" thickBot="1">
       <c r="A80" s="232"/>
       <c r="B80" s="188">
         <f>SUM(C2:C75)</f>
         <v>34</v>
       </c>
       <c r="C80" s="189" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="D80" s="190">
         <f>SUM(B81)</f>
         <v>0</v>
       </c>
       <c r="E80" s="191"/>
-      <c r="F80" s="254">
+      <c r="F80" s="255">
         <f>SUM(D80,E81)</f>
         <v>0</v>
       </c>
-      <c r="G80" s="255"/>
+      <c r="G80" s="256"/>
       <c r="H80" s="192"/>
       <c r="I80" s="123"/>
       <c r="J80" s="123"/>
@@ -14423,7 +14689,7 @@
       <c r="CM80" s="68"/>
       <c r="CN80" s="68"/>
     </row>
-    <row r="81" spans="1:92" ht="31" thickTop="1" thickBot="1">
+    <row r="81" spans="1:92" ht="30.75" thickTop="1" thickBot="1">
       <c r="A81" s="232"/>
       <c r="B81" s="173">
         <f>SUM(D2)</f>
@@ -14432,8 +14698,8 @@
       <c r="C81" s="174"/>
       <c r="D81" s="175"/>
       <c r="E81" s="176"/>
-      <c r="F81" s="256"/>
-      <c r="G81" s="257"/>
+      <c r="F81" s="248"/>
+      <c r="G81" s="249"/>
       <c r="H81" s="182"/>
       <c r="I81" s="123"/>
       <c r="J81" s="123"/>
@@ -14441,7 +14707,7 @@
       <c r="L81" s="123"/>
       <c r="M81" s="123"/>
       <c r="N81" s="183" t="s">
-        <v>109</v>
+        <v>158</v>
       </c>
       <c r="O81" s="172"/>
       <c r="P81" s="172"/>
@@ -14451,15 +14717,15 @@
       <c r="T81" s="123"/>
       <c r="U81" s="123"/>
       <c r="V81" s="184" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="W81" s="123"/>
-      <c r="X81" s="258">
+      <c r="X81" s="252">
         <f>F79</f>
         <v>61.5</v>
       </c>
-      <c r="Y81" s="259"/>
-      <c r="Z81" s="260"/>
+      <c r="Y81" s="253"/>
+      <c r="Z81" s="254"/>
       <c r="AA81" s="172"/>
       <c r="AB81" s="172"/>
       <c r="AC81" s="172"/>
@@ -14527,24 +14793,24 @@
       <c r="CM81" s="68"/>
       <c r="CN81" s="68"/>
     </row>
-    <row r="82" spans="1:92" ht="31" thickTop="1" thickBot="1">
+    <row r="82" spans="1:92" ht="30.75" thickTop="1" thickBot="1">
       <c r="A82" s="231" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="B82" s="173">
         <f>SUM(E2)</f>
         <v>0</v>
       </c>
       <c r="C82" s="179" t="s">
-        <v>110</v>
+        <v>159</v>
       </c>
       <c r="D82" s="180"/>
       <c r="E82" s="181"/>
-      <c r="F82" s="261">
+      <c r="F82" s="250">
         <f>SUM(F80-B83)</f>
         <v>0</v>
       </c>
-      <c r="G82" s="262"/>
+      <c r="G82" s="251"/>
       <c r="H82" s="196"/>
       <c r="I82" s="197"/>
       <c r="J82" s="197"/>
@@ -14631,7 +14897,7 @@
       <c r="CM82" s="68"/>
       <c r="CN82" s="68"/>
     </row>
-    <row r="83" spans="1:92" ht="31" thickTop="1" thickBot="1">
+    <row r="83" spans="1:92" ht="30.75" thickTop="1" thickBot="1">
       <c r="A83" s="231">
         <f>SUM(A84:B84)</f>
         <v>0</v>
@@ -14643,8 +14909,8 @@
       <c r="C83" s="198"/>
       <c r="D83" s="199"/>
       <c r="E83" s="199"/>
-      <c r="F83" s="263"/>
-      <c r="G83" s="264"/>
+      <c r="F83" s="257"/>
+      <c r="G83" s="258"/>
       <c r="H83" s="200"/>
       <c r="I83" s="123"/>
       <c r="J83" s="123"/>
@@ -14652,7 +14918,7 @@
       <c r="L83" s="123"/>
       <c r="M83" s="123"/>
       <c r="N83" s="185" t="s">
-        <v>111</v>
+        <v>160</v>
       </c>
       <c r="O83" s="172"/>
       <c r="P83" s="172"/>
@@ -14662,15 +14928,15 @@
       <c r="T83" s="89"/>
       <c r="U83" s="89"/>
       <c r="V83" s="184" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="W83" s="123"/>
-      <c r="X83" s="265">
+      <c r="X83" s="259">
         <f>A79</f>
         <v>34</v>
       </c>
-      <c r="Y83" s="266"/>
-      <c r="Z83" s="267"/>
+      <c r="Y83" s="260"/>
+      <c r="Z83" s="261"/>
       <c r="AA83" s="172"/>
       <c r="AB83" s="172"/>
       <c r="AC83" s="172"/>
@@ -14738,19 +15004,19 @@
       <c r="CM83" s="68"/>
       <c r="CN83" s="68"/>
     </row>
-    <row r="84" spans="1:92" ht="30.5" thickTop="1" thickBot="1">
+    <row r="84" spans="1:92" ht="30.4" thickTop="1" thickBot="1">
       <c r="A84" s="232"/>
       <c r="B84" s="188">
         <f>SUM(C2)</f>
         <v>0</v>
       </c>
       <c r="C84" s="189" t="s">
-        <v>112</v>
+        <v>161</v>
       </c>
       <c r="D84" s="190"/>
       <c r="E84" s="190"/>
-      <c r="F84" s="243"/>
-      <c r="G84" s="244"/>
+      <c r="F84" s="262"/>
+      <c r="G84" s="263"/>
       <c r="H84" s="192"/>
       <c r="I84" s="123"/>
       <c r="J84" s="123"/>
@@ -14831,20 +15097,20 @@
       <c r="CG84" s="68"/>
       <c r="CH84" s="68"/>
       <c r="CI84" s="68"/>
-      <c r="CJ84" s="245"/>
-      <c r="CK84" s="245"/>
+      <c r="CJ84" s="264"/>
+      <c r="CK84" s="264"/>
       <c r="CL84" s="170"/>
       <c r="CM84" s="170"/>
       <c r="CN84" s="170"/>
     </row>
-    <row r="85" spans="1:92" ht="31" thickTop="1" thickBot="1">
+    <row r="85" spans="1:92" ht="30.75" thickTop="1" thickBot="1">
       <c r="A85" s="232"/>
       <c r="B85" s="201"/>
       <c r="C85" s="202"/>
       <c r="D85" s="203"/>
       <c r="E85" s="203"/>
-      <c r="F85" s="246"/>
-      <c r="G85" s="247"/>
+      <c r="F85" s="265"/>
+      <c r="G85" s="266"/>
       <c r="H85" s="204"/>
       <c r="I85" s="123"/>
       <c r="J85" s="123"/>
@@ -14852,7 +15118,7 @@
       <c r="L85" s="123"/>
       <c r="M85" s="185"/>
       <c r="N85" s="185" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="O85" s="172"/>
       <c r="P85" s="172"/>
@@ -14862,15 +15128,15 @@
       <c r="T85" s="123"/>
       <c r="U85" s="123"/>
       <c r="V85" s="184" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="W85" s="123"/>
-      <c r="X85" s="248">
+      <c r="X85" s="267">
         <f>F77/29</f>
         <v>10.327586206896552</v>
       </c>
-      <c r="Y85" s="249"/>
-      <c r="Z85" s="250"/>
+      <c r="Y85" s="268"/>
+      <c r="Z85" s="269"/>
       <c r="AA85" s="172"/>
       <c r="AB85" s="172"/>
       <c r="AC85" s="172"/>
@@ -14938,9 +15204,9 @@
       <c r="CM85" s="123"/>
       <c r="CN85" s="68"/>
     </row>
-    <row r="86" spans="1:92" ht="30.5" thickTop="1" thickBot="1">
+    <row r="86" spans="1:92" ht="30.4" thickTop="1" thickBot="1">
       <c r="A86" s="233" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
       <c r="B86" s="206"/>
       <c r="C86" s="207"/>
@@ -14952,8 +15218,8 @@
         <f>SUM(E78,E81)</f>
         <v>0</v>
       </c>
-      <c r="F86" s="251"/>
-      <c r="G86" s="252"/>
+      <c r="F86" s="270"/>
+      <c r="G86" s="271"/>
       <c r="H86" s="209"/>
       <c r="I86" s="210"/>
       <c r="J86" s="210"/>
@@ -15030,8 +15296,8 @@
       <c r="CC86" s="213"/>
       <c r="CD86" s="213"/>
       <c r="CE86" s="213"/>
-      <c r="CF86" s="253"/>
-      <c r="CG86" s="253"/>
+      <c r="CF86" s="272"/>
+      <c r="CG86" s="272"/>
       <c r="CH86" s="213"/>
       <c r="CI86" s="213"/>
       <c r="CJ86" s="210"/>
@@ -15042,36 +15308,18 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="AB76:AC76"/>
-    <mergeCell ref="AF76:AG76"/>
-    <mergeCell ref="BD1:BE1"/>
-    <mergeCell ref="BH1:BI1"/>
-    <mergeCell ref="BL1:BM1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AR1:AS1"/>
-    <mergeCell ref="AV1:AW1"/>
-    <mergeCell ref="AZ1:BA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="L76:M76"/>
-    <mergeCell ref="P76:Q76"/>
-    <mergeCell ref="T76:U76"/>
-    <mergeCell ref="X76:Y76"/>
-    <mergeCell ref="AZ76:BA76"/>
-    <mergeCell ref="BD76:BE76"/>
-    <mergeCell ref="CB1:CC1"/>
-    <mergeCell ref="CF1:CG1"/>
-    <mergeCell ref="CJ1:CK1"/>
-    <mergeCell ref="BP1:BQ1"/>
-    <mergeCell ref="BT1:BU1"/>
-    <mergeCell ref="BX1:BY1"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="CJ84:CK84"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="X85:Z85"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="CF86:CG86"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="X81:Z81"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="X83:Z83"/>
     <mergeCell ref="CF76:CG76"/>
     <mergeCell ref="CJ76:CK76"/>
     <mergeCell ref="F77:G77"/>
@@ -15088,19 +15336,38 @@
     <mergeCell ref="AN76:AO76"/>
     <mergeCell ref="AR76:AS76"/>
     <mergeCell ref="AV76:AW76"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="X81:Z81"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="X83:Z83"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="CJ84:CK84"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="X85:Z85"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="CF86:CG86"/>
+    <mergeCell ref="CB1:CC1"/>
+    <mergeCell ref="CF1:CG1"/>
+    <mergeCell ref="CJ1:CK1"/>
+    <mergeCell ref="BP1:BQ1"/>
+    <mergeCell ref="BT1:BU1"/>
+    <mergeCell ref="BX1:BY1"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="L76:M76"/>
+    <mergeCell ref="P76:Q76"/>
+    <mergeCell ref="T76:U76"/>
+    <mergeCell ref="X76:Y76"/>
+    <mergeCell ref="AB76:AC76"/>
+    <mergeCell ref="AF76:AG76"/>
+    <mergeCell ref="BD1:BE1"/>
+    <mergeCell ref="BH1:BI1"/>
+    <mergeCell ref="BL1:BM1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AV1:AW1"/>
+    <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AZ76:BA76"/>
+    <mergeCell ref="BD76:BE76"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="X1:Y1"/>
   </mergeCells>
+  <phoneticPr fontId="44" type="noConversion"/>
   <conditionalFormatting sqref="A2:A71">
     <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="0.25">
       <formula>NOT(ISERROR(SEARCH("0.25",A2)))</formula>
@@ -15204,4 +15471,175 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010012193468DF0E114C90D6B864AF83EA25" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a9a8afa2ca449fd2a2602a1bfa10f9fc">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4514e19c-d173-4674-b6f8-fb25fe19c2d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ca60eb4a5dad36f1e5ab3f9b5e434ea0" ns2:_="">
+    <xsd:import namespace="4514e19c-d173-4674-b6f8-fb25fe19c2d6"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="4514e19c-d173-4674-b6f8-fb25fe19c2d6" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{784D9DDC-31CD-419D-8659-60E4B9EACB1C}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C72E05E-51D6-4AC3-AA4D-77A2934354FF}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0956FEFB-4112-4C8A-9B97-5027CBB05F55}"/>
 </file>
</xml_diff>